<commit_message>
updated electrode mapping to ignore incorrect settings
</commit_message>
<xml_diff>
--- a/defaults/electrode_mapping_short_cables.xlsx
+++ b/defaults/electrode_mapping_short_cables.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S\Documents\Projects\NeuraViPeR\NeuraViPeR_once_worked\NeuraViPeR\ViperBoxInterface\defaults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98011C5C-EEC8-42A8-B349-A4A763EB7CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2E36AC-F3A3-40B5-AEC1-01EA1AEB9D2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{BBC9133A-47E8-4183-A3D2-0E13C727BDE7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{BBC9133A-47E8-4183-A3D2-0E13C727BDE7}"/>
   </bookViews>
   <sheets>
     <sheet name="chan2el" sheetId="1" r:id="rId1"/>
     <sheet name="probeelec_to_asic_el_pad" sheetId="6" r:id="rId2"/>
     <sheet name="low_res" sheetId="7" r:id="rId3"/>
-    <sheet name="emulator_mapping" sheetId="8" r:id="rId4"/>
+    <sheet name="emulator_mapping" sheetId="8" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">emulator_mapping!$A$1:$K$61</definedName>
@@ -2832,7 +2832,7 @@
   <dimension ref="A1:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+      <selection activeCell="P41" sqref="P41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
@@ -2895,20 +2895,20 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="22">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="B2" s="22">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="C2" s="22">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E2" s="27">
         <f>IFERROR(VLOOKUP($B2,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="F2" s="27" t="str">
         <f>IFERROR(VLOOKUP($B2,chan2el!$C$3:$F$66,4,FALSE),"")</f>
@@ -2916,127 +2916,127 @@
       </c>
       <c r="G2" s="27">
         <f>IFERROR(VLOOKUP($B2,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="H2" s="27" t="str">
         <f>IFERROR(VLOOKUP($B2,chan2el!$E$3:$F$66,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="I2" s="25">
-        <f>G2</f>
-        <v>32</v>
+        <f>E2</f>
+        <v>54</v>
       </c>
       <c r="J2" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I2),2,1))) - 64-5</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K2" s="23" t="str">
         <f>IF(COUNTIF($I$1:I1,I2)&gt;0, "Duplicate", "Unique")</f>
         <v>Unique</v>
       </c>
       <c r="L2">
-        <f>I2</f>
-        <v>32</v>
+        <f>IF(AND(K2="Unique",AND(I2&gt;=1,I2&lt;=64)),I2,"")</f>
+        <v>54</v>
       </c>
       <c r="M2" s="25">
-        <f ca="1">IF(K2="Unique",J2,"")</f>
-        <v>2</v>
+        <f ca="1">IF(AND(K2="Unique",AND(I2&gt;=1,I2&lt;=64)),J2,"")</f>
+        <v>0</v>
       </c>
       <c r="N2">
-        <f>IF(K2="Unique",C2,"")</f>
-        <v>5</v>
+        <f>IF(AND(K2="Unique",AND(I2&gt;=1,I2&lt;=64)),A2,"")</f>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="22">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="B3" s="22">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C3" s="22">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="D3" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="27" t="str">
         <f>IFERROR(VLOOKUP($B3,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>64</v>
-      </c>
-      <c r="F3" s="27" t="str">
+        <v/>
+      </c>
+      <c r="F3" s="27">
         <f>IFERROR(VLOOKUP($B3,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="G3" s="27">
+        <v>53</v>
+      </c>
+      <c r="G3" s="27" t="str">
         <f>IFERROR(VLOOKUP($B3,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>53</v>
-      </c>
-      <c r="H3" s="27" t="str">
+        <v/>
+      </c>
+      <c r="H3" s="27">
         <f>IFERROR(VLOOKUP($B3,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="I3" s="25">
-        <f>G3</f>
-        <v>53</v>
+        <v>49</v>
+      </c>
+      <c r="I3">
+        <f>H3</f>
+        <v>49</v>
       </c>
       <c r="J3" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I3),2,1))) - 64-5</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K3" s="23" t="str">
         <f>IF(COUNTIF($I$1:I2,I3)&gt;0, "Duplicate", "Unique")</f>
         <v>Unique</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L61" si="0">I3</f>
-        <v>53</v>
+        <f t="shared" ref="L3:L61" si="0">IF(AND(K3="Unique",AND(I3&gt;=1,I3&lt;=64)),I3,"")</f>
+        <v>49</v>
       </c>
       <c r="M3" s="25">
-        <f ca="1">IF(K3="Unique",J3,"")</f>
+        <f t="shared" ref="M3:M61" ca="1" si="1">IF(AND(K3="Unique",AND(I3&gt;=1,I3&lt;=64)),J3,"")</f>
+        <v>3</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N61" si="2">IF(AND(K3="Unique",AND(I3&gt;=1,I3&lt;=64)),A3,"")</f>
         <v>2</v>
-      </c>
-      <c r="N3">
-        <f t="shared" ref="N3:N61" si="1">IF(K3="Unique",C3,"")</f>
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="22">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="B4" s="22">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="C4" s="22">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="D4" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="27">
+      <c r="E4" s="27" t="str">
         <f>IFERROR(VLOOKUP($B4,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>40</v>
-      </c>
-      <c r="F4" s="27" t="str">
+        <v/>
+      </c>
+      <c r="F4" s="27">
         <f>IFERROR(VLOOKUP($B4,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="G4" s="27">
+        <v>47</v>
+      </c>
+      <c r="G4" s="27" t="str">
         <f>IFERROR(VLOOKUP($B4,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>36</v>
-      </c>
-      <c r="H4" s="27" t="str">
+        <v/>
+      </c>
+      <c r="H4" s="27">
         <f>IFERROR(VLOOKUP($B4,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="I4" s="25">
-        <f>G4</f>
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="I4">
+        <f>F4</f>
+        <v>47</v>
       </c>
       <c r="J4" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I4),2,1))) - 64-5</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K4" s="23" t="str">
         <f>IF(COUNTIF($I$1:I3,I4)&gt;0, "Duplicate", "Unique")</f>
@@ -3044,53 +3044,53 @@
       </c>
       <c r="L4">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="M4" s="25">
-        <f t="shared" ref="M4:M61" ca="1" si="2">IF(K4="Unique",J4,"")</f>
-        <v>2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
       </c>
       <c r="N4">
-        <f t="shared" si="1"/>
-        <v>9</v>
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="22">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="B5" s="22">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="C5" s="22">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="D5" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="27" t="str">
         <f>IFERROR(VLOOKUP($B5,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>56</v>
-      </c>
-      <c r="F5" s="27" t="str">
+        <v/>
+      </c>
+      <c r="F5" s="27">
         <f>IFERROR(VLOOKUP($B5,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="G5" s="27">
+        <v>45</v>
+      </c>
+      <c r="G5" s="27" t="str">
         <f>IFERROR(VLOOKUP($B5,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>52</v>
-      </c>
-      <c r="H5" s="27" t="str">
+        <v/>
+      </c>
+      <c r="H5" s="27">
         <f>IFERROR(VLOOKUP($B5,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v/>
+        <v>40</v>
       </c>
       <c r="I5">
-        <f>E5</f>
-        <v>56</v>
+        <f>F5</f>
+        <v>45</v>
       </c>
       <c r="J5" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I5),2,1))) - 64-5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" s="23" t="str">
         <f>IF(COUNTIF($I$1:I4,I5)&gt;0, "Duplicate", "Unique")</f>
@@ -3098,53 +3098,53 @@
       </c>
       <c r="L5">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="M5" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
       </c>
       <c r="N5">
-        <f t="shared" si="1"/>
-        <v>11</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="22">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="B6" s="22">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="C6" s="22">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="27" t="str">
+        <v>19</v>
+      </c>
+      <c r="E6" s="27">
         <f>IFERROR(VLOOKUP($B6,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="F6" s="27">
+        <v>46</v>
+      </c>
+      <c r="F6" s="27" t="str">
         <f>IFERROR(VLOOKUP($B6,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v>37</v>
-      </c>
-      <c r="G6" s="27" t="str">
+        <v/>
+      </c>
+      <c r="G6" s="27">
         <f>IFERROR(VLOOKUP($B6,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="H6" s="27">
+        <v>39</v>
+      </c>
+      <c r="H6" s="27" t="str">
         <f>IFERROR(VLOOKUP($B6,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v>33</v>
-      </c>
-      <c r="I6" s="25">
-        <f>H6</f>
-        <v>33</v>
+        <v/>
+      </c>
+      <c r="I6">
+        <f>E6</f>
+        <v>46</v>
       </c>
       <c r="J6" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I6),2,1))) - 64-5</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K6" s="23" t="str">
         <f>IF(COUNTIF($I$1:I5,I6)&gt;0, "Duplicate", "Unique")</f>
@@ -3152,87 +3152,87 @@
       </c>
       <c r="L6">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="M6" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="N6">
-        <f t="shared" si="1"/>
-        <v>13</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="22">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="B7" s="22">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C7" s="22">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="27" t="str">
+        <v>19</v>
+      </c>
+      <c r="E7" s="27">
         <f>IFERROR(VLOOKUP($B7,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="F7" s="27">
+        <v>57</v>
+      </c>
+      <c r="F7" s="27" t="str">
         <f>IFERROR(VLOOKUP($B7,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v>36</v>
+        <v/>
       </c>
       <c r="G7" s="27">
         <f>IFERROR(VLOOKUP($B7,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="H7" s="27" t="str">
         <f>IFERROR(VLOOKUP($B7,chan2el!$E$3:$F$66,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="I7" s="25">
-        <f>F7</f>
-        <v>36</v>
+        <f>E7</f>
+        <v>57</v>
       </c>
       <c r="J7" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I7),2,1))) - 64-5</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" s="23" t="str">
         <f>IF(COUNTIF($I$1:I6,I7)&gt;0, "Duplicate", "Unique")</f>
-        <v>Duplicate</v>
+        <v>Unique</v>
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="M7" s="25" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N7" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>57</v>
+      </c>
+      <c r="M7" s="25">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="22">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="B8" s="22">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="C8" s="22">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E8" s="27">
         <f>IFERROR(VLOOKUP($B8,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="F8" s="27" t="str">
         <f>IFERROR(VLOOKUP($B8,chan2el!$C$3:$F$66,4,FALSE),"")</f>
@@ -3240,19 +3240,19 @@
       </c>
       <c r="G8" s="27">
         <f>IFERROR(VLOOKUP($B8,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="H8" s="27" t="str">
         <f>IFERROR(VLOOKUP($B8,chan2el!$E$3:$F$66,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="I8">
-        <f>G8</f>
-        <v>54</v>
+        <f>E8</f>
+        <v>24</v>
       </c>
       <c r="J8" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I8),2,1))) - 64-5</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K8" s="23" t="str">
         <f>IF(COUNTIF($I$1:I7,I8)&gt;0, "Duplicate", "Unique")</f>
@@ -3260,33 +3260,33 @@
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="M8" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="N8">
-        <f t="shared" si="1"/>
-        <v>17</v>
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="22">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="B9" s="22">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="C9" s="22">
+        <v>12</v>
+      </c>
+      <c r="D9" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>22</v>
       </c>
       <c r="E9" s="27">
         <f>IFERROR(VLOOKUP($B9,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="F9" s="27" t="str">
         <f>IFERROR(VLOOKUP($B9,chan2el!$C$3:$F$66,4,FALSE),"")</f>
@@ -3294,19 +3294,19 @@
       </c>
       <c r="G9" s="27">
         <f>IFERROR(VLOOKUP($B9,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="H9" s="27" t="str">
         <f>IFERROR(VLOOKUP($B9,chan2el!$E$3:$F$66,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="I9">
-        <f>E9</f>
-        <v>22</v>
+      <c r="I9" s="25">
+        <f>G9</f>
+        <v>40</v>
       </c>
       <c r="J9" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I9),2,1))) - 64-5</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K9" s="23" t="str">
         <f>IF(COUNTIF($I$1:I8,I9)&gt;0, "Duplicate", "Unique")</f>
@@ -3314,37 +3314,37 @@
       </c>
       <c r="L9">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="M9" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
       </c>
       <c r="N9">
-        <f t="shared" si="1"/>
-        <v>19</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="22">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="B10" s="22">
-        <v>4</v>
+        <v>104</v>
       </c>
       <c r="C10" s="22">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D10" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="27" t="str">
         <f>IFERROR(VLOOKUP($B10,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>4</v>
-      </c>
-      <c r="F10" s="27" t="str">
+        <v/>
+      </c>
+      <c r="F10" s="27">
         <f>IFERROR(VLOOKUP($B10,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v/>
+        <v>40</v>
       </c>
       <c r="G10" s="27" t="str">
         <f>IFERROR(VLOOKUP($B10,chan2el!$D$3:$F$66,3,FALSE),"")</f>
@@ -3352,15 +3352,15 @@
       </c>
       <c r="H10" s="27">
         <f>IFERROR(VLOOKUP($B10,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v>25</v>
-      </c>
-      <c r="I10">
-        <f>E10</f>
-        <v>4</v>
+        <v>36</v>
+      </c>
+      <c r="I10" s="25">
+        <f>H10</f>
+        <v>36</v>
       </c>
       <c r="J10" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I10),2,1))) - 64-5</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K10" s="23" t="str">
         <f>IF(COUNTIF($I$1:I9,I10)&gt;0, "Duplicate", "Unique")</f>
@@ -3368,53 +3368,53 @@
       </c>
       <c r="L10">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="M10" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
       </c>
       <c r="N10">
-        <f t="shared" si="1"/>
-        <v>21</v>
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="22">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="B11" s="22">
-        <v>5</v>
+        <v>123</v>
       </c>
       <c r="C11" s="22">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="D11" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E11" s="27" t="str">
         <f>IFERROR(VLOOKUP($B11,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>5</v>
-      </c>
-      <c r="F11" s="27" t="str">
+        <v/>
+      </c>
+      <c r="F11" s="27">
         <f>IFERROR(VLOOKUP($B11,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="G11" s="27">
+        <v>62</v>
+      </c>
+      <c r="G11" s="27" t="str">
         <f>IFERROR(VLOOKUP($B11,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>1</v>
-      </c>
-      <c r="H11" s="27" t="str">
+        <v/>
+      </c>
+      <c r="H11" s="27">
         <f>IFERROR(VLOOKUP($B11,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v/>
+        <v>55</v>
       </c>
       <c r="I11">
-        <f>E11</f>
-        <v>5</v>
+        <f>F11</f>
+        <v>62</v>
       </c>
       <c r="J11" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I11),2,1))) - 64-5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" s="23" t="str">
         <f>IF(COUNTIF($I$1:I10,I11)&gt;0, "Duplicate", "Unique")</f>
@@ -3422,53 +3422,53 @@
       </c>
       <c r="L11">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="M11" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
       </c>
       <c r="N11">
-        <f t="shared" si="1"/>
-        <v>23</v>
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="22">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="B12" s="22">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="C12" s="22">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="D12" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E12" s="27" t="str">
         <f>IFERROR(VLOOKUP($B12,chan2el!$B$3:$F$66,5,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="F12" s="27">
+        <f>IFERROR(VLOOKUP($B12,chan2el!$C$3:$F$66,4,FALSE),"")</f>
         <v>55</v>
       </c>
-      <c r="F12" s="27" t="str">
-        <f>IFERROR(VLOOKUP($B12,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="G12" s="27">
+      <c r="G12" s="27" t="str">
         <f>IFERROR(VLOOKUP($B12,chan2el!$D$3:$F$66,3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="H12" s="27">
+        <f>IFERROR(VLOOKUP($B12,chan2el!$E$3:$F$66,2,FALSE),"")</f>
         <v>51</v>
       </c>
-      <c r="H12" s="27" t="str">
-        <f>IFERROR(VLOOKUP($B12,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="I12">
-        <f>E12</f>
-        <v>55</v>
+      <c r="I12" s="25">
+        <f>H12</f>
+        <v>51</v>
       </c>
       <c r="J12" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I12),2,1))) - 64-5</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K12" s="23" t="str">
         <f>IF(COUNTIF($I$1:I11,I12)&gt;0, "Duplicate", "Unique")</f>
@@ -3476,53 +3476,53 @@
       </c>
       <c r="L12">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="M12" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
       </c>
       <c r="N12">
-        <f t="shared" si="1"/>
-        <v>24</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="22">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="B13" s="22">
-        <v>73</v>
+        <v>105</v>
       </c>
       <c r="C13" s="22">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="D13" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E13" s="27" t="str">
         <f>IFERROR(VLOOKUP($B13,chan2el!$B$3:$F$66,5,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="F13" s="27">
+        <f>IFERROR(VLOOKUP($B13,chan2el!$C$3:$F$66,4,FALSE),"")</f>
         <v>48</v>
       </c>
-      <c r="F13" s="27" t="str">
-        <f>IFERROR(VLOOKUP($B13,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="G13" s="27">
+      <c r="G13" s="27" t="str">
         <f>IFERROR(VLOOKUP($B13,chan2el!$D$3:$F$66,3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="H13" s="27">
+        <f>IFERROR(VLOOKUP($B13,chan2el!$E$3:$F$66,2,FALSE),"")</f>
         <v>37</v>
       </c>
-      <c r="H13" s="27" t="str">
-        <f>IFERROR(VLOOKUP($B13,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v/>
-      </c>
       <c r="I13">
-        <f>E13</f>
+        <f>F13</f>
         <v>48</v>
       </c>
       <c r="J13" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I13),2,1))) - 64-5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" s="23" t="str">
         <f>IF(COUNTIF($I$1:I12,I13)&gt;0, "Duplicate", "Unique")</f>
@@ -3533,38 +3533,38 @@
         <v>48</v>
       </c>
       <c r="M13" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
       </c>
       <c r="N13">
-        <f t="shared" si="1"/>
-        <v>25</v>
+        <f t="shared" si="2"/>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="22">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="B14" s="22">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C14" s="22">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="27" t="str">
+        <v>19</v>
+      </c>
+      <c r="E14" s="27">
         <f>IFERROR(VLOOKUP($B14,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="F14" s="27">
+        <v>62</v>
+      </c>
+      <c r="F14" s="27" t="str">
         <f>IFERROR(VLOOKUP($B14,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v>35</v>
+        <v/>
       </c>
       <c r="G14" s="27">
         <f>IFERROR(VLOOKUP($B14,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H14" s="27" t="str">
         <f>IFERROR(VLOOKUP($B14,chan2el!$E$3:$F$66,2,FALSE),"")</f>
@@ -3572,7 +3572,7 @@
       </c>
       <c r="I14" s="25">
         <f>G14</f>
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J14" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I14),2,1))) - 64-5</f>
@@ -3584,53 +3584,53 @@
       </c>
       <c r="L14">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="M14" s="25">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>2</v>
       </c>
       <c r="N14">
-        <f t="shared" si="1"/>
-        <v>26</v>
+        <f t="shared" si="2"/>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="22">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="B15" s="22">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="C15" s="22">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="27" t="str">
+        <v>19</v>
+      </c>
+      <c r="E15" s="27">
         <f>IFERROR(VLOOKUP($B15,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="F15" s="27">
+        <v>53</v>
+      </c>
+      <c r="F15" s="27" t="str">
         <f>IFERROR(VLOOKUP($B15,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v>38</v>
-      </c>
-      <c r="G15" s="27" t="str">
+        <v/>
+      </c>
+      <c r="G15" s="27">
         <f>IFERROR(VLOOKUP($B15,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="H15" s="27">
+        <v>49</v>
+      </c>
+      <c r="H15" s="27" t="str">
         <f>IFERROR(VLOOKUP($B15,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v>34</v>
-      </c>
-      <c r="I15">
-        <f>H15</f>
-        <v>34</v>
+        <v/>
+      </c>
+      <c r="I15" s="25">
+        <f>E15</f>
+        <v>53</v>
       </c>
       <c r="J15" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I15),2,1))) - 64-5</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K15" s="23" t="str">
         <f>IF(COUNTIF($I$1:I14,I15)&gt;0, "Duplicate", "Unique")</f>
@@ -3638,53 +3638,53 @@
       </c>
       <c r="L15">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="M15" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="N15">
-        <f t="shared" si="1"/>
-        <v>27</v>
+        <f t="shared" si="2"/>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="22">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="B16" s="22">
-        <v>71</v>
+        <v>120</v>
       </c>
       <c r="C16" s="22">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="D16" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E16" s="27" t="str">
         <f>IFERROR(VLOOKUP($B16,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>39</v>
-      </c>
-      <c r="F16" s="27" t="str">
+        <v/>
+      </c>
+      <c r="F16" s="27">
         <f>IFERROR(VLOOKUP($B16,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="G16" s="27">
+        <v>56</v>
+      </c>
+      <c r="G16" s="27" t="str">
         <f>IFERROR(VLOOKUP($B16,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>35</v>
-      </c>
-      <c r="H16" s="27" t="str">
+        <v/>
+      </c>
+      <c r="H16" s="27">
         <f>IFERROR(VLOOKUP($B16,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v/>
+        <v>52</v>
       </c>
       <c r="I16">
-        <f>G16</f>
-        <v>35</v>
+        <f>F16</f>
+        <v>56</v>
       </c>
       <c r="J16" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I16),2,1))) - 64-5</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K16" s="23" t="str">
         <f>IF(COUNTIF($I$1:I15,I16)&gt;0, "Duplicate", "Unique")</f>
@@ -3692,53 +3692,53 @@
       </c>
       <c r="L16">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="M16" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
       </c>
       <c r="N16">
-        <f t="shared" si="1"/>
-        <v>28</v>
+        <f t="shared" si="2"/>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="22">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="B17" s="22">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="C17" s="22">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="D17" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="27">
+      <c r="E17" s="27" t="str">
         <f>IFERROR(VLOOKUP($B17,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>47</v>
-      </c>
-      <c r="F17" s="27" t="str">
+        <v/>
+      </c>
+      <c r="F17" s="27">
         <f>IFERROR(VLOOKUP($B17,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="G17" s="27">
+        <v>54</v>
+      </c>
+      <c r="G17" s="27" t="str">
         <f>IFERROR(VLOOKUP($B17,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>38</v>
-      </c>
-      <c r="H17" s="27" t="str">
+        <v/>
+      </c>
+      <c r="H17" s="27">
         <f>IFERROR(VLOOKUP($B17,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v/>
+        <v>50</v>
       </c>
       <c r="I17">
-        <f>E17</f>
-        <v>47</v>
+        <f>H17</f>
+        <v>50</v>
       </c>
       <c r="J17" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I17),2,1))) - 64-5</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K17" s="23" t="str">
         <f>IF(COUNTIF($I$1:I16,I17)&gt;0, "Duplicate", "Unique")</f>
@@ -3746,37 +3746,37 @@
       </c>
       <c r="L17">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M17" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
       </c>
       <c r="N17">
-        <f t="shared" si="1"/>
-        <v>29</v>
+        <f t="shared" si="2"/>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="22">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B18" s="22">
-        <v>108</v>
+        <v>1</v>
       </c>
       <c r="C18" s="22">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D18" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="27" t="str">
+      <c r="E18" s="27">
         <f>IFERROR(VLOOKUP($B18,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="F18" s="27">
+        <v>1</v>
+      </c>
+      <c r="F18" s="27" t="str">
         <f>IFERROR(VLOOKUP($B18,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v>45</v>
+        <v/>
       </c>
       <c r="G18" s="27" t="str">
         <f>IFERROR(VLOOKUP($B18,chan2el!$D$3:$F$66,3,FALSE),"")</f>
@@ -3784,15 +3784,15 @@
       </c>
       <c r="H18" s="27">
         <f>IFERROR(VLOOKUP($B18,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="I18">
-        <f>F18</f>
-        <v>45</v>
+        <f>H18</f>
+        <v>28</v>
       </c>
       <c r="J18" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I18),2,1))) - 64-5</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K18" s="23" t="str">
         <f>IF(COUNTIF($I$1:I17,I18)&gt;0, "Duplicate", "Unique")</f>
@@ -3800,53 +3800,53 @@
       </c>
       <c r="L18">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="M18" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
       </c>
       <c r="N18">
-        <f t="shared" si="1"/>
-        <v>36</v>
+        <f t="shared" si="2"/>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="22">
+        <v>18</v>
+      </c>
+      <c r="B19" s="22">
         <v>19</v>
       </c>
-      <c r="B19" s="22">
-        <v>121</v>
-      </c>
       <c r="C19" s="22">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D19" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="27" t="str">
+      <c r="E19" s="27">
         <f>IFERROR(VLOOKUP($B19,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="F19" s="27">
+        <v>19</v>
+      </c>
+      <c r="F19" s="27" t="str">
         <f>IFERROR(VLOOKUP($B19,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v>64</v>
-      </c>
-      <c r="G19" s="27" t="str">
+        <v/>
+      </c>
+      <c r="G19" s="27">
         <f>IFERROR(VLOOKUP($B19,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="H19" s="27">
+        <v>10</v>
+      </c>
+      <c r="H19" s="27" t="str">
         <f>IFERROR(VLOOKUP($B19,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v>53</v>
+        <v/>
       </c>
       <c r="I19">
-        <f>F19</f>
-        <v>64</v>
+        <f>E19</f>
+        <v>19</v>
       </c>
       <c r="J19" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I19),2,1))) - 64-5</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19" s="23" t="str">
         <f>IF(COUNTIF($I$1:I18,I19)&gt;0, "Duplicate", "Unique")</f>
@@ -3854,26 +3854,26 @@
       </c>
       <c r="L19">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="M19" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="N19">
-        <f t="shared" si="1"/>
-        <v>37</v>
+        <f t="shared" si="2"/>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="22">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B20" s="22">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="C20" s="22">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D20" s="22" t="s">
         <v>22</v>
@@ -3884,7 +3884,7 @@
       </c>
       <c r="F20" s="27">
         <f>IFERROR(VLOOKUP($B20,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="G20" s="27" t="str">
         <f>IFERROR(VLOOKUP($B20,chan2el!$D$3:$F$66,3,FALSE),"")</f>
@@ -3892,69 +3892,69 @@
       </c>
       <c r="H20" s="27">
         <f>IFERROR(VLOOKUP($B20,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v>36</v>
-      </c>
-      <c r="I20" s="25">
-        <f>H20</f>
-        <v>36</v>
+        <v>53</v>
+      </c>
+      <c r="I20">
+        <f>F20</f>
+        <v>64</v>
       </c>
       <c r="J20" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I20),2,1))) - 64-5</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K20" s="23" t="str">
         <f>IF(COUNTIF($I$1:I19,I20)&gt;0, "Duplicate", "Unique")</f>
-        <v>Duplicate</v>
+        <v>Unique</v>
       </c>
       <c r="L20">
         <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="M20" s="25" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N20" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>64</v>
+      </c>
+      <c r="M20" s="25">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="2"/>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="22">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B21" s="22">
-        <v>122</v>
+        <v>93</v>
       </c>
       <c r="C21" s="22">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="27" t="str">
+        <v>19</v>
+      </c>
+      <c r="E21" s="27">
         <f>IFERROR(VLOOKUP($B21,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="F21" s="27">
+        <v>60</v>
+      </c>
+      <c r="F21" s="27" t="str">
         <f>IFERROR(VLOOKUP($B21,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v>63</v>
-      </c>
-      <c r="G21" s="27" t="str">
+        <v/>
+      </c>
+      <c r="G21" s="27">
         <f>IFERROR(VLOOKUP($B21,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="H21" s="27">
+        <v>64</v>
+      </c>
+      <c r="H21" s="27" t="str">
         <f>IFERROR(VLOOKUP($B21,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v>54</v>
+        <v/>
       </c>
       <c r="I21">
-        <f>F21</f>
-        <v>63</v>
+        <f>E21</f>
+        <v>60</v>
       </c>
       <c r="J21" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I21),2,1))) - 64-5</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K21" s="23" t="str">
         <f>IF(COUNTIF($I$1:I20,I21)&gt;0, "Duplicate", "Unique")</f>
@@ -3962,29 +3962,29 @@
       </c>
       <c r="L21">
         <f t="shared" si="0"/>
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="M21" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="N21">
-        <f t="shared" si="1"/>
-        <v>39</v>
+        <f t="shared" si="2"/>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="22">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B22" s="22">
-        <v>123</v>
+        <v>53</v>
       </c>
       <c r="C22" s="22">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E22" s="27" t="str">
         <f>IFERROR(VLOOKUP($B22,chan2el!$B$3:$F$66,5,FALSE),"")</f>
@@ -3992,7 +3992,7 @@
       </c>
       <c r="F22" s="27">
         <f>IFERROR(VLOOKUP($B22,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="G22" s="27" t="str">
         <f>IFERROR(VLOOKUP($B22,chan2el!$D$3:$F$66,3,FALSE),"")</f>
@@ -4000,11 +4000,11 @@
       </c>
       <c r="H22" s="27">
         <f>IFERROR(VLOOKUP($B22,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="I22">
         <f>F22</f>
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="J22" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I22),2,1))) - 64-5</f>
@@ -4016,33 +4016,33 @@
       </c>
       <c r="L22">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="M22" s="25">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="N22">
-        <f t="shared" si="1"/>
-        <v>40</v>
+        <f t="shared" si="2"/>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="22">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B23" s="22">
+        <v>84</v>
+      </c>
+      <c r="C23" s="22">
+        <v>10</v>
+      </c>
+      <c r="D23" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="C23" s="22">
-        <v>42</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>22</v>
       </c>
       <c r="E23" s="27">
         <f>IFERROR(VLOOKUP($B23,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="F23" s="27" t="str">
         <f>IFERROR(VLOOKUP($B23,chan2el!$C$3:$F$66,4,FALSE),"")</f>
@@ -4050,7 +4050,7 @@
       </c>
       <c r="G23" s="27">
         <f>IFERROR(VLOOKUP($B23,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="H23" s="27" t="str">
         <f>IFERROR(VLOOKUP($B23,chan2el!$E$3:$F$66,2,FALSE),"")</f>
@@ -4058,7 +4058,7 @@
       </c>
       <c r="I23">
         <f>E23</f>
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="J23" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I23),2,1))) - 64-5</f>
@@ -4070,91 +4070,91 @@
       </c>
       <c r="L23">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="M23" s="25">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="N23">
-        <f t="shared" si="1"/>
-        <v>42</v>
+        <f t="shared" si="2"/>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" s="22">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B24" s="22">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="C24" s="22">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="27" t="str">
+        <v>19</v>
+      </c>
+      <c r="E24" s="27">
         <f>IFERROR(VLOOKUP($B24,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="F24" s="27">
+        <v>38</v>
+      </c>
+      <c r="F24" s="27" t="str">
         <f>IFERROR(VLOOKUP($B24,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v>47</v>
-      </c>
-      <c r="G24" s="27" t="str">
+        <v/>
+      </c>
+      <c r="G24" s="27">
         <f>IFERROR(VLOOKUP($B24,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="H24" s="27">
+        <v>34</v>
+      </c>
+      <c r="H24" s="27" t="str">
         <f>IFERROR(VLOOKUP($B24,chan2el!$E$3:$F$66,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="I24">
+        <f>E24</f>
         <v>38</v>
-      </c>
-      <c r="I24">
-        <f>F24</f>
-        <v>47</v>
       </c>
       <c r="J24" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I24),2,1))) - 64-5</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K24" s="23" t="str">
         <f>IF(COUNTIF($I$1:I23,I24)&gt;0, "Duplicate", "Unique")</f>
-        <v>Duplicate</v>
+        <v>Unique</v>
       </c>
       <c r="L24">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="M24" s="25" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N24" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>38</v>
+      </c>
+      <c r="M24" s="25">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="2"/>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" s="22">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B25" s="22">
-        <v>1</v>
+        <v>122</v>
       </c>
       <c r="C25" s="22">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D25" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="27">
+      <c r="E25" s="27" t="str">
         <f>IFERROR(VLOOKUP($B25,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>1</v>
-      </c>
-      <c r="F25" s="27" t="str">
+        <v/>
+      </c>
+      <c r="F25" s="27">
         <f>IFERROR(VLOOKUP($B25,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v/>
+        <v>63</v>
       </c>
       <c r="G25" s="27" t="str">
         <f>IFERROR(VLOOKUP($B25,chan2el!$D$3:$F$66,3,FALSE),"")</f>
@@ -4162,15 +4162,15 @@
       </c>
       <c r="H25" s="27">
         <f>IFERROR(VLOOKUP($B25,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="I25">
-        <f>H25</f>
-        <v>28</v>
+        <f>F25</f>
+        <v>63</v>
       </c>
       <c r="J25" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I25),2,1))) - 64-5</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K25" s="23" t="str">
         <f>IF(COUNTIF($I$1:I24,I25)&gt;0, "Duplicate", "Unique")</f>
@@ -4178,53 +4178,53 @@
       </c>
       <c r="L25">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="M25" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
       </c>
       <c r="N25">
-        <f t="shared" si="1"/>
-        <v>46</v>
+        <f t="shared" si="2"/>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" s="22">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B26" s="22">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="C26" s="22">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E26" s="27" t="str">
+        <v>19</v>
+      </c>
+      <c r="E26" s="27">
         <f>IFERROR(VLOOKUP($B26,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="F26" s="27">
+        <v>61</v>
+      </c>
+      <c r="F26" s="27" t="str">
         <f>IFERROR(VLOOKUP($B26,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v>53</v>
-      </c>
-      <c r="G26" s="27" t="str">
+        <v/>
+      </c>
+      <c r="G26" s="27">
         <f>IFERROR(VLOOKUP($B26,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="H26" s="27">
+        <v>56</v>
+      </c>
+      <c r="H26" s="27" t="str">
         <f>IFERROR(VLOOKUP($B26,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v>49</v>
+        <v/>
       </c>
       <c r="I26">
-        <f>H26</f>
-        <v>49</v>
+        <f>E26</f>
+        <v>61</v>
       </c>
       <c r="J26" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I26),2,1))) - 64-5</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K26" s="23" t="str">
         <f>IF(COUNTIF($I$1:I25,I26)&gt;0, "Duplicate", "Unique")</f>
@@ -4232,26 +4232,26 @@
       </c>
       <c r="L26">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="M26" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="N26">
-        <f t="shared" si="1"/>
-        <v>48</v>
+        <f t="shared" si="2"/>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" s="22">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B27" s="22">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="C27" s="22">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="D27" s="22" t="s">
         <v>22</v>
@@ -4262,7 +4262,7 @@
       </c>
       <c r="F27" s="27">
         <f>IFERROR(VLOOKUP($B27,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="G27" s="27" t="str">
         <f>IFERROR(VLOOKUP($B27,chan2el!$D$3:$F$66,3,FALSE),"")</f>
@@ -4270,15 +4270,15 @@
       </c>
       <c r="H27" s="27">
         <f>IFERROR(VLOOKUP($B27,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v>50</v>
-      </c>
-      <c r="I27">
-        <f>H27</f>
-        <v>50</v>
+        <v>35</v>
+      </c>
+      <c r="I27" s="25">
+        <f>F27</f>
+        <v>39</v>
       </c>
       <c r="J27" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I27),2,1))) - 64-5</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K27" s="23" t="str">
         <f>IF(COUNTIF($I$1:I26,I27)&gt;0, "Duplicate", "Unique")</f>
@@ -4286,53 +4286,53 @@
       </c>
       <c r="L27">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="M27" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
       </c>
       <c r="N27">
-        <f t="shared" si="1"/>
-        <v>50</v>
+        <f t="shared" si="2"/>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" s="22">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B28" s="22">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="C28" s="22">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E28" s="27" t="str">
+        <v>19</v>
+      </c>
+      <c r="E28" s="27">
         <f>IFERROR(VLOOKUP($B28,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="F28" s="27">
+        <v>37</v>
+      </c>
+      <c r="F28" s="27" t="str">
         <f>IFERROR(VLOOKUP($B28,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v>55</v>
-      </c>
-      <c r="G28" s="27" t="str">
+        <v/>
+      </c>
+      <c r="G28" s="27">
         <f>IFERROR(VLOOKUP($B28,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="H28" s="27">
+        <v>33</v>
+      </c>
+      <c r="H28" s="27" t="str">
         <f>IFERROR(VLOOKUP($B28,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v>51</v>
-      </c>
-      <c r="I28" s="25">
-        <f>H28</f>
-        <v>51</v>
+        <v/>
+      </c>
+      <c r="I28">
+        <f>E28</f>
+        <v>37</v>
       </c>
       <c r="J28" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I28),2,1))) - 64-5</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K28" s="23" t="str">
         <f>IF(COUNTIF($I$1:I27,I28)&gt;0, "Duplicate", "Unique")</f>
@@ -4340,145 +4340,145 @@
       </c>
       <c r="L28">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="M28" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="N28">
-        <f t="shared" si="1"/>
-        <v>52</v>
+        <f t="shared" si="2"/>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" s="22">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B29" s="22">
-        <v>120</v>
+        <v>77</v>
       </c>
       <c r="C29" s="22">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E29" s="27" t="str">
+        <v>19</v>
+      </c>
+      <c r="E29" s="27">
         <f>IFERROR(VLOOKUP($B29,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="F29" s="27">
+        <v>44</v>
+      </c>
+      <c r="F29" s="27" t="str">
         <f>IFERROR(VLOOKUP($B29,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v>56</v>
-      </c>
-      <c r="G29" s="27" t="str">
+        <v/>
+      </c>
+      <c r="G29" s="27">
         <f>IFERROR(VLOOKUP($B29,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="H29" s="27">
+        <v>48</v>
+      </c>
+      <c r="H29" s="27" t="str">
         <f>IFERROR(VLOOKUP($B29,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v>52</v>
+        <v/>
       </c>
       <c r="I29">
-        <f>F29</f>
-        <v>56</v>
+        <f>E29</f>
+        <v>44</v>
       </c>
       <c r="J29" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I29),2,1))) - 64-5</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K29" s="23" t="str">
         <f>IF(COUNTIF($I$1:I28,I29)&gt;0, "Duplicate", "Unique")</f>
-        <v>Duplicate</v>
+        <v>Unique</v>
       </c>
       <c r="L29">
         <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-      <c r="M29" s="25" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N29" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>44</v>
+      </c>
+      <c r="M29" s="25">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="2"/>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" s="22">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="B30" s="22">
-        <v>105</v>
+        <v>18</v>
       </c>
       <c r="C30" s="22">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D30" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E30" s="27" t="str">
+      <c r="E30" s="27">
         <f>IFERROR(VLOOKUP($B30,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="F30" s="27">
+        <v>18</v>
+      </c>
+      <c r="F30" s="27" t="str">
         <f>IFERROR(VLOOKUP($B30,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v>48</v>
-      </c>
-      <c r="G30" s="27" t="str">
+        <v/>
+      </c>
+      <c r="G30" s="27">
         <f>IFERROR(VLOOKUP($B30,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="H30" s="27">
+        <v>11</v>
+      </c>
+      <c r="H30" s="27" t="str">
         <f>IFERROR(VLOOKUP($B30,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v>37</v>
+        <v/>
       </c>
       <c r="I30">
-        <f>F30</f>
-        <v>48</v>
+        <f>E30</f>
+        <v>18</v>
       </c>
       <c r="J30" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I30),2,1))) - 64-5</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K30" s="23" t="str">
         <f>IF(COUNTIF($I$1:I29,I30)&gt;0, "Duplicate", "Unique")</f>
-        <v>Duplicate</v>
+        <v>Unique</v>
       </c>
       <c r="L30">
         <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="M30" s="25" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N30" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>18</v>
+      </c>
+      <c r="M30" s="25">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="2"/>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" s="22">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B31" s="22">
-        <v>103</v>
+        <v>68</v>
       </c>
       <c r="C31" s="22">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E31" s="27" t="str">
+        <v>19</v>
+      </c>
+      <c r="E31" s="27">
         <f>IFERROR(VLOOKUP($B31,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="F31" s="27">
+        <v>36</v>
+      </c>
+      <c r="F31" s="27" t="str">
         <f>IFERROR(VLOOKUP($B31,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v>39</v>
+        <v/>
       </c>
       <c r="G31" s="27" t="str">
         <f>IFERROR(VLOOKUP($B31,chan2el!$D$3:$F$66,3,FALSE),"")</f>
@@ -4486,11 +4486,11 @@
       </c>
       <c r="H31" s="27">
         <f>IFERROR(VLOOKUP($B31,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v>35</v>
-      </c>
-      <c r="I31" t="str">
+        <v>57</v>
+      </c>
+      <c r="I31" s="25">
         <f>E31</f>
-        <v/>
+        <v>36</v>
       </c>
       <c r="J31" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I31),2,1))) - 64-5</f>
@@ -4498,37 +4498,37 @@
       </c>
       <c r="K31" s="23" t="str">
         <f>IF(COUNTIF($I$1:I30,I31)&gt;0, "Duplicate", "Unique")</f>
-        <v>Unique</v>
+        <v>Duplicate</v>
       </c>
       <c r="L31" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M31" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N31">
+      <c r="M31" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>58</v>
+        <v/>
+      </c>
+      <c r="N31" t="str">
+        <f t="shared" si="2"/>
+        <v/>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" s="22">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B32" s="22">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="C32" s="22">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E32" s="27">
         <f>IFERROR(VLOOKUP($B32,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="F32" s="27" t="str">
         <f>IFERROR(VLOOKUP($B32,chan2el!$C$3:$F$66,4,FALSE),"")</f>
@@ -4536,19 +4536,19 @@
       </c>
       <c r="G32" s="27">
         <f>IFERROR(VLOOKUP($B32,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="H32" s="27" t="str">
         <f>IFERROR(VLOOKUP($B32,chan2el!$E$3:$F$66,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="I32">
-        <f>E32</f>
-        <v>18</v>
+        <f>G32</f>
+        <v>43</v>
       </c>
       <c r="J32" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I32),2,1))) - 64-5</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K32" s="23" t="str">
         <f>IF(COUNTIF($I$1:I31,I32)&gt;0, "Duplicate", "Unique")</f>
@@ -4556,33 +4556,33 @@
       </c>
       <c r="L32">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="M32" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
       </c>
       <c r="N32">
-        <f t="shared" si="1"/>
-        <v>60</v>
+        <f t="shared" si="2"/>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" s="22">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B33" s="22">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C33" s="22">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="D33" s="22" t="s">
         <v>19</v>
       </c>
       <c r="E33" s="27">
         <f>IFERROR(VLOOKUP($B33,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F33" s="27" t="str">
         <f>IFERROR(VLOOKUP($B33,chan2el!$C$3:$F$66,4,FALSE),"")</f>
@@ -4590,7 +4590,7 @@
       </c>
       <c r="G33" s="27">
         <f>IFERROR(VLOOKUP($B33,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="H33" s="27" t="str">
         <f>IFERROR(VLOOKUP($B33,chan2el!$E$3:$F$66,2,FALSE),"")</f>
@@ -4598,7 +4598,7 @@
       </c>
       <c r="I33">
         <f>E33</f>
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="J33" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I33),2,1))) - 64-5</f>
@@ -4606,37 +4606,37 @@
       </c>
       <c r="K33" s="23" t="str">
         <f>IF(COUNTIF($I$1:I32,I33)&gt;0, "Duplicate", "Unique")</f>
-        <v>Unique</v>
-      </c>
-      <c r="L33">
+        <v>Duplicate</v>
+      </c>
+      <c r="L33" t="str">
         <f t="shared" si="0"/>
-        <v>61</v>
-      </c>
-      <c r="M33" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N33">
+        <v/>
+      </c>
+      <c r="M33" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v/>
+      </c>
+      <c r="N33" t="str">
+        <f t="shared" si="2"/>
+        <v/>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" s="22">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="B34" s="22">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C34" s="22">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="D34" s="22" t="s">
         <v>19</v>
       </c>
       <c r="E34" s="27">
         <f>IFERROR(VLOOKUP($B34,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F34" s="27" t="str">
         <f>IFERROR(VLOOKUP($B34,chan2el!$C$3:$F$66,4,FALSE),"")</f>
@@ -4644,69 +4644,69 @@
       </c>
       <c r="G34" s="27">
         <f>IFERROR(VLOOKUP($B34,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H34" s="27" t="str">
         <f>IFERROR(VLOOKUP($B34,chan2el!$E$3:$F$66,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="I34" s="25">
-        <f>E34</f>
-        <v>54</v>
+        <f>G34</f>
+        <v>47</v>
       </c>
       <c r="J34" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I34),2,1))) - 64-5</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K34" s="23" t="str">
         <f>IF(COUNTIF($I$1:I33,I34)&gt;0, "Duplicate", "Unique")</f>
         <v>Duplicate</v>
       </c>
-      <c r="L34">
+      <c r="L34" t="str">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v/>
       </c>
       <c r="M34" s="25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="N34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" s="22">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B35" s="22">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C35" s="22">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="D35" s="22" t="s">
         <v>19</v>
       </c>
       <c r="E35" s="27">
         <f>IFERROR(VLOOKUP($B35,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="F35" s="27" t="str">
         <f>IFERROR(VLOOKUP($B35,chan2el!$C$3:$F$66,4,FALSE),"")</f>
         <v/>
       </c>
-      <c r="G35" s="27">
+      <c r="G35" s="27" t="str">
         <f>IFERROR(VLOOKUP($B35,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>39</v>
-      </c>
-      <c r="H35" s="27" t="str">
+        <v/>
+      </c>
+      <c r="H35" s="27">
         <f>IFERROR(VLOOKUP($B35,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v/>
+        <v>59</v>
       </c>
       <c r="I35">
         <f>E35</f>
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="J35" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I35),2,1))) - 64-5</f>
@@ -4718,87 +4718,87 @@
       </c>
       <c r="L35">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="M35" s="25">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="N35">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f t="shared" si="2"/>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" s="22">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B36" s="22">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="C36" s="22">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="E36" s="27">
+        <v>22</v>
+      </c>
+      <c r="E36" s="27" t="str">
         <f>IFERROR(VLOOKUP($B36,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>60</v>
-      </c>
-      <c r="F36" s="27" t="str">
+        <v/>
+      </c>
+      <c r="F36" s="27">
         <f>IFERROR(VLOOKUP($B36,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v/>
+        <v>36</v>
       </c>
       <c r="G36" s="27">
         <f>IFERROR(VLOOKUP($B36,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="H36" s="27" t="str">
         <f>IFERROR(VLOOKUP($B36,chan2el!$E$3:$F$66,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="I36">
-        <f>E36</f>
-        <v>60</v>
+      <c r="I36" s="25">
+        <f>F36</f>
+        <v>36</v>
       </c>
       <c r="J36" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I36),2,1))) - 64-5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K36" s="23" t="str">
         <f>IF(COUNTIF($I$1:I35,I36)&gt;0, "Duplicate", "Unique")</f>
-        <v>Unique</v>
-      </c>
-      <c r="L36">
+        <v>Duplicate</v>
+      </c>
+      <c r="L36" t="str">
         <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="M36" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N36">
+        <v/>
+      </c>
+      <c r="M36" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v/>
+      </c>
+      <c r="N36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" s="22">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B37" s="22">
-        <v>77</v>
+        <v>22</v>
       </c>
       <c r="C37" s="22">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E37" s="27">
         <f>IFERROR(VLOOKUP($B37,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="F37" s="27" t="str">
         <f>IFERROR(VLOOKUP($B37,chan2el!$C$3:$F$66,4,FALSE),"")</f>
@@ -4806,7 +4806,7 @@
       </c>
       <c r="G37" s="27">
         <f>IFERROR(VLOOKUP($B37,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="H37" s="27" t="str">
         <f>IFERROR(VLOOKUP($B37,chan2el!$E$3:$F$66,2,FALSE),"")</f>
@@ -4814,7 +4814,7 @@
       </c>
       <c r="I37">
         <f>E37</f>
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="J37" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I37),2,1))) - 64-5</f>
@@ -4826,33 +4826,33 @@
       </c>
       <c r="L37">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="M37" s="25">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="N37">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <f t="shared" si="2"/>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" s="22">
+        <v>37</v>
+      </c>
+      <c r="B38" s="22">
+        <v>5</v>
+      </c>
+      <c r="C38" s="22">
+        <v>23</v>
+      </c>
+      <c r="D38" s="22" t="s">
         <v>22</v>
-      </c>
-      <c r="B38" s="22">
-        <v>84</v>
-      </c>
-      <c r="C38" s="22">
-        <v>10</v>
-      </c>
-      <c r="D38" s="22" t="s">
-        <v>19</v>
       </c>
       <c r="E38" s="27">
         <f>IFERROR(VLOOKUP($B38,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="F38" s="27" t="str">
         <f>IFERROR(VLOOKUP($B38,chan2el!$C$3:$F$66,4,FALSE),"")</f>
@@ -4860,7 +4860,7 @@
       </c>
       <c r="G38" s="27">
         <f>IFERROR(VLOOKUP($B38,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="H38" s="27" t="str">
         <f>IFERROR(VLOOKUP($B38,chan2el!$E$3:$F$66,2,FALSE),"")</f>
@@ -4868,7 +4868,7 @@
       </c>
       <c r="I38">
         <f>E38</f>
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="J38" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I38),2,1))) - 64-5</f>
@@ -4880,33 +4880,33 @@
       </c>
       <c r="L38">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="M38" s="25">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="N38">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39" s="22">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="B39" s="22">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C39" s="22">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E39" s="27">
         <f>IFERROR(VLOOKUP($B39,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F39" s="27" t="str">
         <f>IFERROR(VLOOKUP($B39,chan2el!$C$3:$F$66,4,FALSE),"")</f>
@@ -4914,15 +4914,15 @@
       </c>
       <c r="G39" s="27">
         <f>IFERROR(VLOOKUP($B39,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H39" s="27" t="str">
         <f>IFERROR(VLOOKUP($B39,chan2el!$E$3:$F$66,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="I39" s="25">
+      <c r="I39">
         <f>G39</f>
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="J39" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I39),2,1))) - 64-5</f>
@@ -4934,87 +4934,87 @@
       </c>
       <c r="L39">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="M39" s="25">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>2</v>
       </c>
       <c r="N39">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40" s="22">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="B40" s="22">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="C40" s="22">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="D40" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="E40" s="27">
+      <c r="E40" s="27" t="str">
         <f>IFERROR(VLOOKUP($B40,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>38</v>
-      </c>
-      <c r="F40" s="27" t="str">
+        <v/>
+      </c>
+      <c r="F40" s="27">
         <f>IFERROR(VLOOKUP($B40,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="G40" s="27">
+        <v>22</v>
+      </c>
+      <c r="G40" s="27" t="str">
         <f>IFERROR(VLOOKUP($B40,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>34</v>
-      </c>
-      <c r="H40" s="27" t="str">
+        <v/>
+      </c>
+      <c r="H40" s="27">
         <f>IFERROR(VLOOKUP($B40,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="I40">
-        <f>E40</f>
-        <v>38</v>
+        <v>18</v>
+      </c>
+      <c r="I40" s="25">
+        <f>H40</f>
+        <v>18</v>
       </c>
       <c r="J40" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I40),2,1))) - 64-5</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K40" s="23" t="str">
         <f>IF(COUNTIF($I$1:I39,I40)&gt;0, "Duplicate", "Unique")</f>
-        <v>Unique</v>
-      </c>
-      <c r="L40">
+        <v>Duplicate</v>
+      </c>
+      <c r="L40" t="str">
         <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="M40" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N40">
+        <v/>
+      </c>
+      <c r="M40" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v/>
+      </c>
+      <c r="N40" t="str">
+        <f t="shared" si="2"/>
+        <v/>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A41" s="22">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="B41" s="22">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C41" s="22">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E41" s="27">
         <f>IFERROR(VLOOKUP($B41,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F41" s="27" t="str">
         <f>IFERROR(VLOOKUP($B41,chan2el!$C$3:$F$66,4,FALSE),"")</f>
@@ -5022,7 +5022,7 @@
       </c>
       <c r="G41" s="27">
         <f>IFERROR(VLOOKUP($B41,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H41" s="27" t="str">
         <f>IFERROR(VLOOKUP($B41,chan2el!$E$3:$F$66,2,FALSE),"")</f>
@@ -5030,7 +5030,7 @@
       </c>
       <c r="I41" s="25">
         <f>G41</f>
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J41" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I41),2,1))) - 64-5</f>
@@ -5040,35 +5040,35 @@
         <f>IF(COUNTIF($I$1:I40,I41)&gt;0, "Duplicate", "Unique")</f>
         <v>Duplicate</v>
       </c>
-      <c r="L41">
+      <c r="L41" t="str">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v/>
       </c>
       <c r="M41" s="25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="N41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42" s="22">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="B42" s="22">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="C42" s="22">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="D42" s="22" t="s">
         <v>19</v>
       </c>
       <c r="E42" s="27">
         <f>IFERROR(VLOOKUP($B42,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="F42" s="27" t="str">
         <f>IFERROR(VLOOKUP($B42,chan2el!$C$3:$F$66,4,FALSE),"")</f>
@@ -5076,15 +5076,15 @@
       </c>
       <c r="G42" s="27">
         <f>IFERROR(VLOOKUP($B42,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="H42" s="27" t="str">
         <f>IFERROR(VLOOKUP($B42,chan2el!$E$3:$F$66,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="I42" s="25">
+      <c r="I42">
         <f>E42</f>
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="J42" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I42),2,1))) - 64-5</f>
@@ -5092,37 +5092,37 @@
       </c>
       <c r="K42" s="23" t="str">
         <f>IF(COUNTIF($I$1:I41,I42)&gt;0, "Duplicate", "Unique")</f>
-        <v>Duplicate</v>
+        <v>Unique</v>
       </c>
       <c r="L42">
         <f t="shared" si="0"/>
-        <v>53</v>
-      </c>
-      <c r="M42" s="25" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N42" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>15</v>
+      </c>
+      <c r="M42" s="25">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="2"/>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A43" s="22">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="B43" s="22">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C43" s="22">
+        <v>5</v>
+      </c>
+      <c r="D43" s="22" t="s">
         <v>22</v>
-      </c>
-      <c r="D43" s="22" t="s">
-        <v>19</v>
       </c>
       <c r="E43" s="27">
         <f>IFERROR(VLOOKUP($B43,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F43" s="27" t="str">
         <f>IFERROR(VLOOKUP($B43,chan2el!$C$3:$F$66,4,FALSE),"")</f>
@@ -5130,19 +5130,19 @@
       </c>
       <c r="G43" s="27">
         <f>IFERROR(VLOOKUP($B43,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="H43" s="27" t="str">
         <f>IFERROR(VLOOKUP($B43,chan2el!$E$3:$F$66,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="I43">
-        <f>E43</f>
-        <v>24</v>
+      <c r="I43" s="25">
+        <f>G43</f>
+        <v>32</v>
       </c>
       <c r="J43" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I43),2,1))) - 64-5</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K43" s="23" t="str">
         <f>IF(COUNTIF($I$1:I42,I43)&gt;0, "Duplicate", "Unique")</f>
@@ -5150,53 +5150,53 @@
       </c>
       <c r="L43">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="M43" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
       </c>
       <c r="N43">
-        <f t="shared" si="1"/>
-        <v>22</v>
+        <f t="shared" si="2"/>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A44" s="22">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="B44" s="22">
-        <v>69</v>
+        <v>99</v>
       </c>
       <c r="C44" s="22">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D44" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="E44" s="27">
+        <v>22</v>
+      </c>
+      <c r="E44" s="27" t="str">
         <f>IFERROR(VLOOKUP($B44,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>37</v>
-      </c>
-      <c r="F44" s="27" t="str">
+        <v/>
+      </c>
+      <c r="F44" s="27">
         <f>IFERROR(VLOOKUP($B44,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v/>
+        <v>35</v>
       </c>
       <c r="G44" s="27">
         <f>IFERROR(VLOOKUP($B44,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="H44" s="27" t="str">
         <f>IFERROR(VLOOKUP($B44,chan2el!$E$3:$F$66,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="I44">
-        <f>E44</f>
-        <v>37</v>
+      <c r="I44" s="25">
+        <f>G44</f>
+        <v>58</v>
       </c>
       <c r="J44" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I44),2,1))) - 64-5</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K44" s="23" t="str">
         <f>IF(COUNTIF($I$1:I43,I44)&gt;0, "Duplicate", "Unique")</f>
@@ -5204,37 +5204,37 @@
       </c>
       <c r="L44">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="M44" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
       </c>
       <c r="N44">
-        <f t="shared" si="1"/>
-        <v>30</v>
+        <f t="shared" si="2"/>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A45" s="22">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B45" s="22">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="C45" s="22">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D45" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="E45" s="27">
+      <c r="E45" s="27" t="str">
         <f>IFERROR(VLOOKUP($B45,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>36</v>
-      </c>
-      <c r="F45" s="27" t="str">
+        <v/>
+      </c>
+      <c r="F45" s="27">
         <f>IFERROR(VLOOKUP($B45,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v/>
+        <v>23</v>
       </c>
       <c r="G45" s="27" t="str">
         <f>IFERROR(VLOOKUP($B45,chan2el!$D$3:$F$66,3,FALSE),"")</f>
@@ -5242,49 +5242,49 @@
       </c>
       <c r="H45" s="27">
         <f>IFERROR(VLOOKUP($B45,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v>57</v>
-      </c>
-      <c r="I45" s="25">
-        <f>E45</f>
-        <v>36</v>
+        <v>19</v>
+      </c>
+      <c r="I45">
+        <f>F45</f>
+        <v>23</v>
       </c>
       <c r="J45" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I45),2,1))) - 64-5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K45" s="23" t="str">
         <f>IF(COUNTIF($I$1:I44,I45)&gt;0, "Duplicate", "Unique")</f>
-        <v>Duplicate</v>
+        <v>Unique</v>
       </c>
       <c r="L45">
         <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="M45" s="25" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N45" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>23</v>
+      </c>
+      <c r="M45" s="25">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="2"/>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A46" s="22">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B46" s="22">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="C46" s="22">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D46" s="22" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E46" s="27">
         <f>IFERROR(VLOOKUP($B46,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="F46" s="27" t="str">
         <f>IFERROR(VLOOKUP($B46,chan2el!$C$3:$F$66,4,FALSE),"")</f>
@@ -5292,73 +5292,73 @@
       </c>
       <c r="G46" s="27">
         <f>IFERROR(VLOOKUP($B46,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="H46" s="27" t="str">
         <f>IFERROR(VLOOKUP($B46,chan2el!$E$3:$F$66,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="I46">
-        <f>E46</f>
-        <v>15</v>
+      <c r="I46" s="25">
+        <f>G46</f>
+        <v>36</v>
       </c>
       <c r="J46" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I46),2,1))) - 64-5</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K46" s="23" t="str">
         <f>IF(COUNTIF($I$1:I45,I46)&gt;0, "Duplicate", "Unique")</f>
-        <v>Unique</v>
-      </c>
-      <c r="L46">
+        <v>Duplicate</v>
+      </c>
+      <c r="L46" t="str">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="M46" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N46">
+        <v/>
+      </c>
+      <c r="M46" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v/>
+      </c>
+      <c r="N46" t="str">
+        <f t="shared" si="2"/>
+        <v/>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A47" s="22">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B47" s="22">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="C47" s="22">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="D47" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="E47" s="27" t="str">
+      <c r="E47" s="27">
         <f>IFERROR(VLOOKUP($B47,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="F47" s="27">
+        <v>41</v>
+      </c>
+      <c r="F47" s="27" t="str">
         <f>IFERROR(VLOOKUP($B47,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v>23</v>
-      </c>
-      <c r="G47" s="27" t="str">
+        <v/>
+      </c>
+      <c r="G47" s="27">
         <f>IFERROR(VLOOKUP($B47,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="H47" s="27">
+        <v>45</v>
+      </c>
+      <c r="H47" s="27" t="str">
         <f>IFERROR(VLOOKUP($B47,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v>19</v>
+        <v/>
       </c>
       <c r="I47">
-        <f>F47</f>
-        <v>23</v>
+        <f>E47</f>
+        <v>41</v>
       </c>
       <c r="J47" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I47),2,1))) - 64-5</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K47" s="23" t="str">
         <f>IF(COUNTIF($I$1:I46,I47)&gt;0, "Duplicate", "Unique")</f>
@@ -5366,33 +5366,33 @@
       </c>
       <c r="L47">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="M47" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="N47">
-        <f t="shared" si="1"/>
-        <v>33</v>
+        <f t="shared" si="2"/>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A48" s="22">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B48" s="22">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C48" s="22">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="D48" s="22" t="s">
         <v>19</v>
       </c>
       <c r="E48" s="27">
         <f>IFERROR(VLOOKUP($B48,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F48" s="27" t="str">
         <f>IFERROR(VLOOKUP($B48,chan2el!$C$3:$F$66,4,FALSE),"")</f>
@@ -5400,69 +5400,69 @@
       </c>
       <c r="G48" s="27">
         <f>IFERROR(VLOOKUP($B48,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H48" s="27" t="str">
         <f>IFERROR(VLOOKUP($B48,chan2el!$E$3:$F$66,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="I48">
-        <f>E48</f>
-        <v>59</v>
+      <c r="I48" s="25">
+        <f>G48</f>
+        <v>62</v>
       </c>
       <c r="J48" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I48),2,1))) - 64-5</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K48" s="23" t="str">
         <f>IF(COUNTIF($I$1:I47,I48)&gt;0, "Duplicate", "Unique")</f>
-        <v>Unique</v>
-      </c>
-      <c r="L48">
+        <v>Duplicate</v>
+      </c>
+      <c r="L48" t="str">
         <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
-      <c r="M48" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N48">
+        <v/>
+      </c>
+      <c r="M48" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v/>
+      </c>
+      <c r="N48" t="str">
+        <f t="shared" si="2"/>
+        <v/>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A49" s="22">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B49" s="22">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C49" s="22">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="D49" s="22" t="s">
         <v>19</v>
       </c>
       <c r="E49" s="27">
         <f>IFERROR(VLOOKUP($B49,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="F49" s="27" t="str">
         <f>IFERROR(VLOOKUP($B49,chan2el!$C$3:$F$66,4,FALSE),"")</f>
         <v/>
       </c>
-      <c r="G49" s="27" t="str">
+      <c r="G49" s="27">
         <f>IFERROR(VLOOKUP($B49,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="H49" s="27">
+        <v>46</v>
+      </c>
+      <c r="H49" s="27" t="str">
         <f>IFERROR(VLOOKUP($B49,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v>58</v>
+        <v/>
       </c>
       <c r="I49">
         <f>E49</f>
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J49" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I49),2,1))) - 64-5</f>
@@ -5470,41 +5470,41 @@
       </c>
       <c r="K49" s="23" t="str">
         <f>IF(COUNTIF($I$1:I48,I49)&gt;0, "Duplicate", "Unique")</f>
-        <v>Duplicate</v>
+        <v>Unique</v>
       </c>
       <c r="L49">
         <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="M49" s="25" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N49" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>42</v>
+      </c>
+      <c r="M49" s="25">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="2"/>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A50" s="22">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B50" s="22">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="C50" s="22">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D50" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="E50" s="27" t="str">
+      <c r="E50" s="27">
         <f>IFERROR(VLOOKUP($B50,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="F50" s="27">
+        <v>33</v>
+      </c>
+      <c r="F50" s="27" t="str">
         <f>IFERROR(VLOOKUP($B50,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v>22</v>
+        <v/>
       </c>
       <c r="G50" s="27" t="str">
         <f>IFERROR(VLOOKUP($B50,chan2el!$D$3:$F$66,3,FALSE),"")</f>
@@ -5512,157 +5512,157 @@
       </c>
       <c r="H50" s="27">
         <f>IFERROR(VLOOKUP($B50,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v>18</v>
-      </c>
-      <c r="I50" s="25">
-        <f>H50</f>
-        <v>18</v>
+        <v>60</v>
+      </c>
+      <c r="I50">
+        <f>E50</f>
+        <v>33</v>
       </c>
       <c r="J50" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I50),2,1))) - 64-5</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K50" s="23" t="str">
         <f>IF(COUNTIF($I$1:I49,I50)&gt;0, "Duplicate", "Unique")</f>
-        <v>Duplicate</v>
+        <v>Unique</v>
       </c>
       <c r="L50">
         <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="M50" s="25" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N50" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>33</v>
+      </c>
+      <c r="M50" s="25">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="2"/>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A51" s="22">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B51" s="22">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="C51" s="22">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="D51" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="E51" s="27">
+        <v>22</v>
+      </c>
+      <c r="E51" s="27" t="str">
         <f>IFERROR(VLOOKUP($B51,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>51</v>
-      </c>
-      <c r="F51" s="27" t="str">
+        <v/>
+      </c>
+      <c r="F51" s="27">
         <f>IFERROR(VLOOKUP($B51,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="G51" s="27">
+        <v>37</v>
+      </c>
+      <c r="G51" s="27" t="str">
         <f>IFERROR(VLOOKUP($B51,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>42</v>
-      </c>
-      <c r="H51" s="27" t="str">
+        <v/>
+      </c>
+      <c r="H51" s="27">
         <f>IFERROR(VLOOKUP($B51,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="I51">
-        <f>E51</f>
-        <v>51</v>
+        <v>33</v>
+      </c>
+      <c r="I51" s="25">
+        <f>H51</f>
+        <v>33</v>
       </c>
       <c r="J51" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I51),2,1))) - 64-5</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K51" s="23" t="str">
         <f>IF(COUNTIF($I$1:I50,I51)&gt;0, "Duplicate", "Unique")</f>
         <v>Duplicate</v>
       </c>
-      <c r="L51">
+      <c r="L51" t="str">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v/>
       </c>
       <c r="M51" s="25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="N51" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A52" s="22">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="B52" s="22">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="C52" s="22">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="D52" s="22" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E52" s="27">
         <f>IFERROR(VLOOKUP($B52,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="F52" s="27" t="str">
         <f>IFERROR(VLOOKUP($B52,chan2el!$C$3:$F$66,4,FALSE),"")</f>
         <v/>
       </c>
-      <c r="G52" s="27" t="str">
+      <c r="G52" s="27">
         <f>IFERROR(VLOOKUP($B52,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="H52" s="27">
+        <v>54</v>
+      </c>
+      <c r="H52" s="27" t="str">
         <f>IFERROR(VLOOKUP($B52,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v>59</v>
+        <v/>
       </c>
       <c r="I52">
-        <f>E52</f>
-        <v>34</v>
+        <f>G52</f>
+        <v>54</v>
       </c>
       <c r="J52" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I52),2,1))) - 64-5</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K52" s="23" t="str">
         <f>IF(COUNTIF($I$1:I51,I52)&gt;0, "Duplicate", "Unique")</f>
         <v>Duplicate</v>
       </c>
-      <c r="L52">
+      <c r="L52" t="str">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v/>
       </c>
       <c r="M52" s="25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="N52" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A53" s="22">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B53" s="22">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="C53" s="22">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="D53" s="22" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E53" s="27">
         <f>IFERROR(VLOOKUP($B53,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="F53" s="27" t="str">
         <f>IFERROR(VLOOKUP($B53,chan2el!$C$3:$F$66,4,FALSE),"")</f>
@@ -5674,11 +5674,11 @@
       </c>
       <c r="H53" s="27">
         <f>IFERROR(VLOOKUP($B53,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="I53">
         <f>E53</f>
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="J53" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I53),2,1))) - 64-5</f>
@@ -5686,37 +5686,37 @@
       </c>
       <c r="K53" s="23" t="str">
         <f>IF(COUNTIF($I$1:I52,I53)&gt;0, "Duplicate", "Unique")</f>
-        <v>Duplicate</v>
+        <v>Unique</v>
       </c>
       <c r="L53">
         <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="M53" s="25" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N53" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>4</v>
+      </c>
+      <c r="M53" s="25">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="2"/>
+        <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A54" s="22">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="B54" s="22">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C54" s="22">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="D54" s="22" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E54" s="27">
         <f>IFERROR(VLOOKUP($B54,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F54" s="27" t="str">
         <f>IFERROR(VLOOKUP($B54,chan2el!$C$3:$F$66,4,FALSE),"")</f>
@@ -5724,53 +5724,53 @@
       </c>
       <c r="G54" s="27">
         <f>IFERROR(VLOOKUP($B54,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="H54" s="27" t="str">
         <f>IFERROR(VLOOKUP($B54,chan2el!$E$3:$F$66,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="I54" s="25">
-        <f>G54</f>
+      <c r="I54">
+        <f>E54</f>
         <v>47</v>
       </c>
       <c r="J54" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I54),2,1))) - 64-5</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K54" s="23" t="str">
         <f>IF(COUNTIF($I$1:I53,I54)&gt;0, "Duplicate", "Unique")</f>
         <v>Duplicate</v>
       </c>
-      <c r="L54">
+      <c r="L54" t="str">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v/>
       </c>
       <c r="M54" s="25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="N54" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A55" s="22">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B55" s="22">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C55" s="22">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D55" s="22" t="s">
         <v>19</v>
       </c>
       <c r="E55" s="27">
         <f>IFERROR(VLOOKUP($B55,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="F55" s="27" t="str">
         <f>IFERROR(VLOOKUP($B55,chan2el!$C$3:$F$66,4,FALSE),"")</f>
@@ -5778,7 +5778,7 @@
       </c>
       <c r="G55" s="27">
         <f>IFERROR(VLOOKUP($B55,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H55" s="27" t="str">
         <f>IFERROR(VLOOKUP($B55,chan2el!$E$3:$F$66,2,FALSE),"")</f>
@@ -5786,7 +5786,7 @@
       </c>
       <c r="I55">
         <f>E55</f>
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="J55" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I55),2,1))) - 64-5</f>
@@ -5794,37 +5794,37 @@
       </c>
       <c r="K55" s="23" t="str">
         <f>IF(COUNTIF($I$1:I54,I55)&gt;0, "Duplicate", "Unique")</f>
-        <v>Unique</v>
-      </c>
-      <c r="L55">
+        <v>Duplicate</v>
+      </c>
+      <c r="L55" t="str">
         <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="M55" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N55">
+        <v/>
+      </c>
+      <c r="M55" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v/>
+      </c>
+      <c r="N55" t="str">
+        <f t="shared" si="2"/>
+        <v/>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A56" s="22">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="B56" s="22">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C56" s="22">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="D56" s="22" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E56" s="27">
         <f>IFERROR(VLOOKUP($B56,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F56" s="27" t="str">
         <f>IFERROR(VLOOKUP($B56,chan2el!$C$3:$F$66,4,FALSE),"")</f>
@@ -5832,15 +5832,15 @@
       </c>
       <c r="G56" s="27">
         <f>IFERROR(VLOOKUP($B56,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="H56" s="27" t="str">
         <f>IFERROR(VLOOKUP($B56,chan2el!$E$3:$F$66,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="I56" s="25">
+      <c r="I56">
         <f>E56</f>
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J56" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I56),2,1))) - 64-5</f>
@@ -5848,57 +5848,57 @@
       </c>
       <c r="K56" s="23" t="str">
         <f>IF(COUNTIF($I$1:I55,I56)&gt;0, "Duplicate", "Unique")</f>
-        <v>Unique</v>
-      </c>
-      <c r="L56">
+        <v>Duplicate</v>
+      </c>
+      <c r="L56" t="str">
         <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="M56" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N56">
+        <v/>
+      </c>
+      <c r="M56" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v/>
+      </c>
+      <c r="N56" t="str">
+        <f t="shared" si="2"/>
+        <v/>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A57" s="22">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="B57" s="22">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="C57" s="22">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="D57" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="E57" s="27" t="str">
+      <c r="E57" s="27">
         <f>IFERROR(VLOOKUP($B57,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="F57" s="27">
+        <v>59</v>
+      </c>
+      <c r="F57" s="27" t="str">
         <f>IFERROR(VLOOKUP($B57,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v>21</v>
-      </c>
-      <c r="G57" s="27" t="str">
+        <v/>
+      </c>
+      <c r="G57" s="27">
         <f>IFERROR(VLOOKUP($B57,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="H57" s="27">
+        <v>63</v>
+      </c>
+      <c r="H57" s="27" t="str">
         <f>IFERROR(VLOOKUP($B57,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v>17</v>
+        <v/>
       </c>
       <c r="I57">
-        <f>F57</f>
-        <v>21</v>
+        <f>E57</f>
+        <v>59</v>
       </c>
       <c r="J57" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I57),2,1))) - 64-5</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K57" s="23" t="str">
         <f>IF(COUNTIF($I$1:I56,I57)&gt;0, "Duplicate", "Unique")</f>
@@ -5906,33 +5906,33 @@
       </c>
       <c r="L57">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="M57" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="N57">
-        <f t="shared" si="1"/>
-        <v>57</v>
+        <f t="shared" si="2"/>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A58" s="22">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="B58" s="22">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="C58" s="22">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="D58" s="22" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E58" s="27">
         <f>IFERROR(VLOOKUP($B58,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="F58" s="27" t="str">
         <f>IFERROR(VLOOKUP($B58,chan2el!$C$3:$F$66,4,FALSE),"")</f>
@@ -5940,7 +5940,7 @@
       </c>
       <c r="G58" s="27">
         <f>IFERROR(VLOOKUP($B58,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="H58" s="27" t="str">
         <f>IFERROR(VLOOKUP($B58,chan2el!$E$3:$F$66,2,FALSE),"")</f>
@@ -5948,7 +5948,7 @@
       </c>
       <c r="I58">
         <f>E58</f>
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="J58" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I58),2,1))) - 64-5</f>
@@ -5958,89 +5958,89 @@
         <f>IF(COUNTIF($I$1:I57,I58)&gt;0, "Duplicate", "Unique")</f>
         <v>Duplicate</v>
       </c>
-      <c r="L58">
+      <c r="L58" t="str">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v/>
       </c>
       <c r="M58" s="25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="N58" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A59" s="22">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B59" s="22">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="C59" s="22">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="E59" s="27">
+        <v>22</v>
+      </c>
+      <c r="E59" s="27" t="str">
         <f>IFERROR(VLOOKUP($B59,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>58</v>
-      </c>
-      <c r="F59" s="27" t="str">
+        <v/>
+      </c>
+      <c r="F59" s="27">
         <f>IFERROR(VLOOKUP($B59,chan2el!$C$3:$F$66,4,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="G59" s="27">
+        <v>38</v>
+      </c>
+      <c r="G59" s="27" t="str">
         <f>IFERROR(VLOOKUP($B59,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>62</v>
-      </c>
-      <c r="H59" s="27" t="str">
+        <v/>
+      </c>
+      <c r="H59" s="27">
         <f>IFERROR(VLOOKUP($B59,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="I59" s="25">
-        <f>G59</f>
-        <v>62</v>
+        <v>34</v>
+      </c>
+      <c r="I59">
+        <f>H59</f>
+        <v>34</v>
       </c>
       <c r="J59" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I59),2,1))) - 64-5</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K59" s="23" t="str">
         <f>IF(COUNTIF($I$1:I58,I59)&gt;0, "Duplicate", "Unique")</f>
         <v>Duplicate</v>
       </c>
-      <c r="L59">
+      <c r="L59" t="str">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v/>
       </c>
       <c r="M59" s="25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="N59" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A60" s="22">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="B60" s="22">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C60" s="22">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E60" s="27">
         <f>IFERROR(VLOOKUP($B60,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F60" s="27" t="str">
         <f>IFERROR(VLOOKUP($B60,chan2el!$C$3:$F$66,4,FALSE),"")</f>
@@ -6048,69 +6048,69 @@
       </c>
       <c r="G60" s="27">
         <f>IFERROR(VLOOKUP($B60,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="H60" s="27" t="str">
         <f>IFERROR(VLOOKUP($B60,chan2el!$E$3:$F$66,2,FALSE),"")</f>
         <v/>
       </c>
       <c r="I60">
-        <f>G60</f>
-        <v>43</v>
+        <f>E60</f>
+        <v>48</v>
       </c>
       <c r="J60" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I60),2,1))) - 64-5</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K60" s="23" t="str">
         <f>IF(COUNTIF($I$1:I59,I60)&gt;0, "Duplicate", "Unique")</f>
-        <v>Unique</v>
-      </c>
-      <c r="L60">
+        <v>Duplicate</v>
+      </c>
+      <c r="L60" t="str">
         <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="M60" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="N60">
+        <v/>
+      </c>
+      <c r="M60" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>63</v>
+        <v/>
+      </c>
+      <c r="N60" t="str">
+        <f t="shared" si="2"/>
+        <v/>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A61" s="22">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B61" s="22">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="C61" s="22">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="D61" s="22" t="s">
         <v>19</v>
       </c>
       <c r="E61" s="27">
         <f>IFERROR(VLOOKUP($B61,chan2el!$B$3:$F$66,5,FALSE),"")</f>
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F61" s="27" t="str">
         <f>IFERROR(VLOOKUP($B61,chan2el!$C$3:$F$66,4,FALSE),"")</f>
         <v/>
       </c>
-      <c r="G61" s="27">
+      <c r="G61" s="27" t="str">
         <f>IFERROR(VLOOKUP($B61,chan2el!$D$3:$F$66,3,FALSE),"")</f>
-        <v>45</v>
-      </c>
-      <c r="H61" s="27" t="str">
+        <v/>
+      </c>
+      <c r="H61" s="27">
         <f>IFERROR(VLOOKUP($B61,chan2el!$E$3:$F$66,2,FALSE),"")</f>
-        <v/>
+        <v>58</v>
       </c>
       <c r="I61">
         <f>E61</f>
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="J61" s="28">
         <f ca="1">CODE(UPPER(MID(_xlfn.FORMULATEXT(I61),2,1))) - 64-5</f>
@@ -6118,25 +6118,25 @@
       </c>
       <c r="K61" s="23" t="str">
         <f>IF(COUNTIF($I$1:I60,I61)&gt;0, "Duplicate", "Unique")</f>
-        <v>Unique</v>
-      </c>
-      <c r="L61">
+        <v>Duplicate</v>
+      </c>
+      <c r="L61" t="str">
         <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="M61" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N61">
+        <v/>
+      </c>
+      <c r="M61" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>64</v>
+        <v/>
+      </c>
+      <c r="N61" t="str">
+        <f t="shared" si="2"/>
+        <v/>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K61" xr:uid="{9B17CD0B-AC8F-4ECC-930B-3416D5CCEB1D}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K61">
-      <sortCondition descending="1" ref="D1:D61"/>
+      <sortCondition ref="A1:A61"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:B61">
@@ -10117,21 +10117,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="f40b0abf-00a2-4b5b-b98d-06c28878d409">
-      <UserInfo>
-        <DisplayName>Piotr Bejm (IC RESOURCES)</DisplayName>
-        <AccountId>39</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="82955996-2c56-4dc5-a205-5349b3b0490a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="eddb54b3-0260-4a74-8bba-cc772719b91b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10383,22 +10374,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="f40b0abf-00a2-4b5b-b98d-06c28878d409">
+      <UserInfo>
+        <DisplayName>Piotr Bejm (IC RESOURCES)</DisplayName>
+        <AccountId>39</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="82955996-2c56-4dc5-a205-5349b3b0490a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="eddb54b3-0260-4a74-8bba-cc772719b91b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29D9ED97-9FFF-4588-8DC9-F5F025F5C220}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC23E6A2-90B8-4860-9A82-94B40C6384C0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f40b0abf-00a2-4b5b-b98d-06c28878d409"/>
-    <ds:schemaRef ds:uri="82955996-2c56-4dc5-a205-5349b3b0490a"/>
-    <ds:schemaRef ds:uri="eddb54b3-0260-4a74-8bba-cc772719b91b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10424,9 +10420,13 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC23E6A2-90B8-4860-9A82-94B40C6384C0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29D9ED97-9FFF-4588-8DC9-F5F025F5C220}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f40b0abf-00a2-4b5b-b98d-06c28878d409"/>
+    <ds:schemaRef ds:uri="82955996-2c56-4dc5-a205-5349b3b0490a"/>
+    <ds:schemaRef ds:uri="eddb54b3-0260-4a74-8bba-cc772719b91b"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update mapping to add extra table for insight
</commit_message>
<xml_diff>
--- a/defaults/electrode_mapping_short_cables.xlsx
+++ b/defaults/electrode_mapping_short_cables.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S\Documents\Projects\NeuraViPeR\NeuraViPeR_once_worked\NeuraViPeR\ViperBoxInterface\defaults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDDD0C9-9B0C-4D67-B5C5-29A137CC06A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8445515B-46A4-4E7C-9A7E-65B2D18D65C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{BBC9133A-47E8-4183-A3D2-0E13C727BDE7}"/>
+    <workbookView xWindow="-23295" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{BBC9133A-47E8-4183-A3D2-0E13C727BDE7}"/>
   </bookViews>
   <sheets>
     <sheet name="chan2el" sheetId="1" r:id="rId1"/>
     <sheet name="probeelec_to_asic_el_pad" sheetId="6" r:id="rId2"/>
     <sheet name="low_res" sheetId="7" r:id="rId3"/>
-    <sheet name="emulator_mapping" sheetId="8" state="hidden" r:id="rId4"/>
+    <sheet name="OS to electr (by IMEC)" sheetId="9" r:id="rId4"/>
+    <sheet name="emulator_mapping" sheetId="8" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">emulator_mapping!$A$1:$K$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">emulator_mapping!$A$1:$K$61</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">probeelec_to_asic_el_pad!$A$1:$K$61</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -187,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="27">
   <si>
     <t>Ch_InP position</t>
   </si>
@@ -257,12 +258,24 @@
   <si>
     <t>T</t>
   </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>ELECTRODE (on probe)</t>
+  </si>
+  <si>
+    <t>Low Resolution</t>
+  </si>
+  <si>
+    <t>High Resolution</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,8 +320,33 @@
       <name val="Gill Sans MT"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Gill Sans MT"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Gill Sans MT"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Gill Sans MT"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Gill Sans MT"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -356,8 +394,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -454,12 +510,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -492,7 +622,175 @@
     <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -861,6 +1159,102 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{364AD23C-F217-4236-8E03-85BE4A901503}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8229600" y="990600"/>
+          <a:ext cx="5391150" cy="676275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" cap="none" spc="0" baseline="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>From this table it can be seen that the amplifiers with lower numbers have fewer probe electrodes connected to them</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" cap="none" spc="0" baseline="0">
+            <a:ln w="0"/>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="dk1">
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1508,12 +1902,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
     </row>
     <row r="2" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
@@ -2831,8 +3225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B17CD0B-AC8F-4ECC-930B-3416D5CCEB1D}">
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
@@ -3139,7 +3533,7 @@
         <v/>
       </c>
       <c r="I6" s="25">
-        <f t="shared" ref="I3:I61" si="5">E6</f>
+        <f t="shared" ref="I6:I57" si="5">E6</f>
         <v>46</v>
       </c>
       <c r="J6" s="28">
@@ -3679,7 +4073,7 @@
         <v>37</v>
       </c>
       <c r="I16" s="25">
-        <f t="shared" ref="I16:I18" si="7">F16</f>
+        <f t="shared" ref="I16:I17" si="7">F16</f>
         <v>48</v>
       </c>
       <c r="J16" s="28">
@@ -4813,7 +5207,7 @@
         <v/>
       </c>
       <c r="I37" s="25">
-        <f t="shared" ref="I36:I37" si="9">G37</f>
+        <f t="shared" ref="I37" si="9">G37</f>
         <v>54</v>
       </c>
       <c r="J37" s="28">
@@ -5947,7 +6341,7 @@
         <v/>
       </c>
       <c r="I58" s="25">
-        <f t="shared" ref="I58:I61" si="12">G58</f>
+        <f t="shared" ref="I58:I60" si="12">G58</f>
         <v>36</v>
       </c>
       <c r="J58" s="28">
@@ -7211,6 +7605,1739 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2058E97E-5E04-473E-AD34-2280327FCF86}">
+  <dimension ref="A1:J67"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:10" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="77" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="79"/>
+      <c r="G1" s="80" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="82"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B2" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="G2" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+    </row>
+    <row r="3" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="29">
+        <v>0</v>
+      </c>
+      <c r="C3" s="29">
+        <v>1</v>
+      </c>
+      <c r="D3" s="29">
+        <v>2</v>
+      </c>
+      <c r="E3" s="29">
+        <v>3</v>
+      </c>
+      <c r="G3" s="29">
+        <v>0</v>
+      </c>
+      <c r="H3" s="29">
+        <v>1</v>
+      </c>
+      <c r="I3" s="29">
+        <v>2</v>
+      </c>
+      <c r="J3" s="29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="30">
+        <v>1</v>
+      </c>
+      <c r="B4" s="42">
+        <v>1</v>
+      </c>
+      <c r="C4" s="43">
+        <v>33</v>
+      </c>
+      <c r="D4" s="43">
+        <v>5</v>
+      </c>
+      <c r="E4" s="64">
+        <v>37</v>
+      </c>
+      <c r="F4" s="83" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="52"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="54">
+        <v>37</v>
+      </c>
+      <c r="J4" s="55"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="30">
+        <v>2</v>
+      </c>
+      <c r="B5" s="44">
+        <v>2</v>
+      </c>
+      <c r="C5" s="45">
+        <v>34</v>
+      </c>
+      <c r="D5" s="45">
+        <v>6</v>
+      </c>
+      <c r="E5" s="65">
+        <v>38</v>
+      </c>
+      <c r="F5" s="84"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="57"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="30">
+        <v>3</v>
+      </c>
+      <c r="B6" s="44">
+        <v>3</v>
+      </c>
+      <c r="C6" s="45">
+        <v>35</v>
+      </c>
+      <c r="D6" s="45">
+        <v>7</v>
+      </c>
+      <c r="E6" s="65">
+        <v>39</v>
+      </c>
+      <c r="F6" s="84"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="29">
+        <v>28</v>
+      </c>
+      <c r="J6" s="57"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="30">
+        <v>4</v>
+      </c>
+      <c r="B7" s="44">
+        <v>4</v>
+      </c>
+      <c r="C7" s="45">
+        <v>36</v>
+      </c>
+      <c r="D7" s="45">
+        <v>8</v>
+      </c>
+      <c r="E7" s="65">
+        <v>40</v>
+      </c>
+      <c r="F7" s="84"/>
+      <c r="G7" s="58">
+        <v>52</v>
+      </c>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="57"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="30">
+        <v>5</v>
+      </c>
+      <c r="B8" s="44">
+        <v>5</v>
+      </c>
+      <c r="C8" s="45">
+        <v>37</v>
+      </c>
+      <c r="D8" s="45">
+        <v>9</v>
+      </c>
+      <c r="E8" s="65">
+        <v>41</v>
+      </c>
+      <c r="F8" s="84"/>
+      <c r="G8" s="58">
+        <v>37</v>
+      </c>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="57"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="30">
+        <v>6</v>
+      </c>
+      <c r="B9" s="44">
+        <v>6</v>
+      </c>
+      <c r="C9" s="45">
+        <v>38</v>
+      </c>
+      <c r="D9" s="45">
+        <v>10</v>
+      </c>
+      <c r="E9" s="65">
+        <v>42</v>
+      </c>
+      <c r="F9" s="84"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="29">
+        <v>41</v>
+      </c>
+      <c r="J9" s="57"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="30">
+        <v>7</v>
+      </c>
+      <c r="B10" s="44">
+        <v>7</v>
+      </c>
+      <c r="C10" s="45">
+        <v>39</v>
+      </c>
+      <c r="D10" s="45">
+        <v>11</v>
+      </c>
+      <c r="E10" s="65">
+        <v>43</v>
+      </c>
+      <c r="F10" s="84"/>
+      <c r="G10" s="58">
+        <v>28</v>
+      </c>
+      <c r="H10" s="50"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="57"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="30">
+        <v>8</v>
+      </c>
+      <c r="B11" s="44">
+        <v>8</v>
+      </c>
+      <c r="C11" s="45">
+        <v>40</v>
+      </c>
+      <c r="D11" s="45">
+        <v>12</v>
+      </c>
+      <c r="E11" s="65">
+        <v>44</v>
+      </c>
+      <c r="F11" s="84"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="57"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="31">
+        <v>9</v>
+      </c>
+      <c r="B12" s="48">
+        <v>16</v>
+      </c>
+      <c r="C12" s="49">
+        <v>48</v>
+      </c>
+      <c r="D12" s="49">
+        <v>20</v>
+      </c>
+      <c r="E12" s="66">
+        <v>52</v>
+      </c>
+      <c r="F12" s="84"/>
+      <c r="G12" s="59">
+        <v>29</v>
+      </c>
+      <c r="H12" s="51"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="60"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="30">
+        <v>10</v>
+      </c>
+      <c r="B13" s="44">
+        <v>15</v>
+      </c>
+      <c r="C13" s="45">
+        <v>47</v>
+      </c>
+      <c r="D13" s="45">
+        <v>19</v>
+      </c>
+      <c r="E13" s="65">
+        <v>51</v>
+      </c>
+      <c r="F13" s="84"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="29">
+        <v>18</v>
+      </c>
+      <c r="J13" s="57"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="30">
+        <v>11</v>
+      </c>
+      <c r="B14" s="44">
+        <v>14</v>
+      </c>
+      <c r="C14" s="45">
+        <v>46</v>
+      </c>
+      <c r="D14" s="45">
+        <v>18</v>
+      </c>
+      <c r="E14" s="65">
+        <v>50</v>
+      </c>
+      <c r="F14" s="84"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="29">
+        <v>26</v>
+      </c>
+      <c r="J14" s="57"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="30">
+        <v>12</v>
+      </c>
+      <c r="B15" s="44">
+        <v>13</v>
+      </c>
+      <c r="C15" s="45">
+        <v>45</v>
+      </c>
+      <c r="D15" s="45">
+        <v>17</v>
+      </c>
+      <c r="E15" s="65">
+        <v>49</v>
+      </c>
+      <c r="F15" s="84"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="57"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="30">
+        <v>13</v>
+      </c>
+      <c r="B16" s="44">
+        <v>12</v>
+      </c>
+      <c r="C16" s="45">
+        <v>44</v>
+      </c>
+      <c r="D16" s="45">
+        <v>16</v>
+      </c>
+      <c r="E16" s="65">
+        <v>48</v>
+      </c>
+      <c r="F16" s="84"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="29">
+        <v>29</v>
+      </c>
+      <c r="J16" s="57"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="30">
+        <v>14</v>
+      </c>
+      <c r="B17" s="44">
+        <v>11</v>
+      </c>
+      <c r="C17" s="45">
+        <v>43</v>
+      </c>
+      <c r="D17" s="45">
+        <v>15</v>
+      </c>
+      <c r="E17" s="65">
+        <v>47</v>
+      </c>
+      <c r="F17" s="84"/>
+      <c r="G17" s="56"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="50"/>
+      <c r="J17" s="57"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" s="30">
+        <v>15</v>
+      </c>
+      <c r="B18" s="44">
+        <v>10</v>
+      </c>
+      <c r="C18" s="45">
+        <v>42</v>
+      </c>
+      <c r="D18" s="45">
+        <v>14</v>
+      </c>
+      <c r="E18" s="65">
+        <v>46</v>
+      </c>
+      <c r="F18" s="84"/>
+      <c r="G18" s="58">
+        <v>41</v>
+      </c>
+      <c r="H18" s="50"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="57"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="31">
+        <v>16</v>
+      </c>
+      <c r="B19" s="44">
+        <v>9</v>
+      </c>
+      <c r="C19" s="45">
+        <v>41</v>
+      </c>
+      <c r="D19" s="45">
+        <v>13</v>
+      </c>
+      <c r="E19" s="65">
+        <v>45</v>
+      </c>
+      <c r="F19" s="84"/>
+      <c r="G19" s="56"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="57"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="31">
+        <v>17</v>
+      </c>
+      <c r="B20" s="44">
+        <v>17</v>
+      </c>
+      <c r="C20" s="45">
+        <v>49</v>
+      </c>
+      <c r="D20" s="45">
+        <v>21</v>
+      </c>
+      <c r="E20" s="65">
+        <v>53</v>
+      </c>
+      <c r="F20" s="84"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="61">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" s="31">
+        <v>18</v>
+      </c>
+      <c r="B21" s="44">
+        <v>18</v>
+      </c>
+      <c r="C21" s="45">
+        <v>50</v>
+      </c>
+      <c r="D21" s="45">
+        <v>22</v>
+      </c>
+      <c r="E21" s="65">
+        <v>54</v>
+      </c>
+      <c r="F21" s="84"/>
+      <c r="G21" s="58">
+        <v>26</v>
+      </c>
+      <c r="H21" s="50"/>
+      <c r="I21" s="50"/>
+      <c r="J21" s="57"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" s="31">
+        <v>19</v>
+      </c>
+      <c r="B22" s="44">
+        <v>19</v>
+      </c>
+      <c r="C22" s="45">
+        <v>51</v>
+      </c>
+      <c r="D22" s="45">
+        <v>23</v>
+      </c>
+      <c r="E22" s="65">
+        <v>55</v>
+      </c>
+      <c r="F22" s="84"/>
+      <c r="G22" s="58">
+        <v>18</v>
+      </c>
+      <c r="H22" s="50"/>
+      <c r="I22" s="50"/>
+      <c r="J22" s="61">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" s="31">
+        <v>20</v>
+      </c>
+      <c r="B23" s="44">
+        <v>20</v>
+      </c>
+      <c r="C23" s="45">
+        <v>52</v>
+      </c>
+      <c r="D23" s="45">
+        <v>24</v>
+      </c>
+      <c r="E23" s="65">
+        <v>56</v>
+      </c>
+      <c r="F23" s="84"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="61">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" s="31">
+        <v>21</v>
+      </c>
+      <c r="B24" s="44">
+        <v>21</v>
+      </c>
+      <c r="C24" s="45">
+        <v>53</v>
+      </c>
+      <c r="D24" s="45">
+        <v>25</v>
+      </c>
+      <c r="E24" s="65">
+        <v>57</v>
+      </c>
+      <c r="F24" s="84"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="29">
+        <v>6</v>
+      </c>
+      <c r="I24" s="50"/>
+      <c r="J24" s="57"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25" s="31">
+        <v>22</v>
+      </c>
+      <c r="B25" s="44">
+        <v>22</v>
+      </c>
+      <c r="C25" s="45">
+        <v>54</v>
+      </c>
+      <c r="D25" s="45">
+        <v>26</v>
+      </c>
+      <c r="E25" s="65">
+        <v>58</v>
+      </c>
+      <c r="F25" s="84"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="57"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" s="31">
+        <v>23</v>
+      </c>
+      <c r="B26" s="44">
+        <v>23</v>
+      </c>
+      <c r="C26" s="45">
+        <v>55</v>
+      </c>
+      <c r="D26" s="45">
+        <v>27</v>
+      </c>
+      <c r="E26" s="65">
+        <v>59</v>
+      </c>
+      <c r="F26" s="84"/>
+      <c r="G26" s="56"/>
+      <c r="H26" s="29">
+        <v>44</v>
+      </c>
+      <c r="I26" s="50"/>
+      <c r="J26" s="57"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27" s="32">
+        <v>24</v>
+      </c>
+      <c r="B27" s="44">
+        <v>24</v>
+      </c>
+      <c r="C27" s="45">
+        <v>56</v>
+      </c>
+      <c r="D27" s="45">
+        <v>28</v>
+      </c>
+      <c r="E27" s="65">
+        <v>60</v>
+      </c>
+      <c r="F27" s="84"/>
+      <c r="G27" s="56"/>
+      <c r="H27" s="29">
+        <v>21</v>
+      </c>
+      <c r="I27" s="29">
+        <v>42</v>
+      </c>
+      <c r="J27" s="57"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" s="32">
+        <v>25</v>
+      </c>
+      <c r="B28" s="44">
+        <v>32</v>
+      </c>
+      <c r="C28" s="45">
+        <v>64</v>
+      </c>
+      <c r="D28" s="45">
+        <v>36</v>
+      </c>
+      <c r="E28" s="65">
+        <v>4</v>
+      </c>
+      <c r="F28" s="84"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="61">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29" s="31">
+        <v>26</v>
+      </c>
+      <c r="B29" s="44">
+        <v>31</v>
+      </c>
+      <c r="C29" s="45">
+        <v>63</v>
+      </c>
+      <c r="D29" s="45">
+        <v>35</v>
+      </c>
+      <c r="E29" s="65">
+        <v>3</v>
+      </c>
+      <c r="F29" s="84"/>
+      <c r="G29" s="56"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="57"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30" s="31">
+        <v>27</v>
+      </c>
+      <c r="B30" s="44">
+        <v>30</v>
+      </c>
+      <c r="C30" s="45">
+        <v>62</v>
+      </c>
+      <c r="D30" s="45">
+        <v>34</v>
+      </c>
+      <c r="E30" s="65">
+        <v>2</v>
+      </c>
+      <c r="F30" s="84"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="50"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="57"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31" s="31">
+        <v>28</v>
+      </c>
+      <c r="B31" s="44">
+        <v>29</v>
+      </c>
+      <c r="C31" s="45">
+        <v>61</v>
+      </c>
+      <c r="D31" s="45">
+        <v>33</v>
+      </c>
+      <c r="E31" s="65">
+        <v>1</v>
+      </c>
+      <c r="F31" s="84"/>
+      <c r="G31" s="58">
+        <v>40</v>
+      </c>
+      <c r="H31" s="50"/>
+      <c r="I31" s="50"/>
+      <c r="J31" s="57"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A32" s="31">
+        <v>29</v>
+      </c>
+      <c r="B32" s="44">
+        <v>28</v>
+      </c>
+      <c r="C32" s="45">
+        <v>60</v>
+      </c>
+      <c r="D32" s="45">
+        <v>32</v>
+      </c>
+      <c r="E32" s="65">
+        <v>64</v>
+      </c>
+      <c r="F32" s="84"/>
+      <c r="G32" s="58">
+        <v>42</v>
+      </c>
+      <c r="H32" s="50"/>
+      <c r="I32" s="50"/>
+      <c r="J32" s="57"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A33" s="31">
+        <v>30</v>
+      </c>
+      <c r="B33" s="44">
+        <v>27</v>
+      </c>
+      <c r="C33" s="45">
+        <v>59</v>
+      </c>
+      <c r="D33" s="45">
+        <v>31</v>
+      </c>
+      <c r="E33" s="65">
+        <v>63</v>
+      </c>
+      <c r="F33" s="84"/>
+      <c r="G33" s="56"/>
+      <c r="H33" s="50"/>
+      <c r="I33" s="50"/>
+      <c r="J33" s="57"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A34" s="30">
+        <v>31</v>
+      </c>
+      <c r="B34" s="44">
+        <v>26</v>
+      </c>
+      <c r="C34" s="45">
+        <v>58</v>
+      </c>
+      <c r="D34" s="45">
+        <v>30</v>
+      </c>
+      <c r="E34" s="65">
+        <v>62</v>
+      </c>
+      <c r="F34" s="84"/>
+      <c r="G34" s="56"/>
+      <c r="H34" s="50"/>
+      <c r="I34" s="50"/>
+      <c r="J34" s="57"/>
+    </row>
+    <row r="35" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="30">
+        <v>32</v>
+      </c>
+      <c r="B35" s="46">
+        <v>25</v>
+      </c>
+      <c r="C35" s="47">
+        <v>57</v>
+      </c>
+      <c r="D35" s="47">
+        <v>29</v>
+      </c>
+      <c r="E35" s="67">
+        <v>61</v>
+      </c>
+      <c r="F35" s="85"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="50"/>
+      <c r="I35" s="29">
+        <v>40</v>
+      </c>
+      <c r="J35" s="57"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A36" s="33">
+        <v>33</v>
+      </c>
+      <c r="B36" s="34">
+        <v>65</v>
+      </c>
+      <c r="C36" s="35">
+        <v>97</v>
+      </c>
+      <c r="D36" s="35">
+        <v>69</v>
+      </c>
+      <c r="E36" s="36">
+        <v>101</v>
+      </c>
+      <c r="F36" s="73" t="s">
+        <v>26</v>
+      </c>
+      <c r="G36" s="68">
+        <v>34</v>
+      </c>
+      <c r="H36" s="53"/>
+      <c r="I36" s="54">
+        <v>27</v>
+      </c>
+      <c r="J36" s="69">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A37" s="33">
+        <v>34</v>
+      </c>
+      <c r="B37" s="37">
+        <v>66</v>
+      </c>
+      <c r="C37" s="71">
+        <v>98</v>
+      </c>
+      <c r="D37" s="71">
+        <v>70</v>
+      </c>
+      <c r="E37" s="38">
+        <v>102</v>
+      </c>
+      <c r="F37" s="74"/>
+      <c r="G37" s="58">
+        <v>54</v>
+      </c>
+      <c r="H37" s="50"/>
+      <c r="I37" s="29">
+        <v>13</v>
+      </c>
+      <c r="J37" s="61">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A38" s="33">
+        <v>35</v>
+      </c>
+      <c r="B38" s="37">
+        <v>67</v>
+      </c>
+      <c r="C38" s="71">
+        <v>99</v>
+      </c>
+      <c r="D38" s="71">
+        <v>71</v>
+      </c>
+      <c r="E38" s="38">
+        <v>103</v>
+      </c>
+      <c r="F38" s="74"/>
+      <c r="G38" s="58">
+        <v>60</v>
+      </c>
+      <c r="H38" s="29">
+        <v>43</v>
+      </c>
+      <c r="I38" s="29">
+        <v>38</v>
+      </c>
+      <c r="J38" s="61">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A39" s="33">
+        <v>36</v>
+      </c>
+      <c r="B39" s="37">
+        <v>68</v>
+      </c>
+      <c r="C39" s="71">
+        <v>100</v>
+      </c>
+      <c r="D39" s="71">
+        <v>72</v>
+      </c>
+      <c r="E39" s="38">
+        <v>104</v>
+      </c>
+      <c r="F39" s="74"/>
+      <c r="G39" s="58">
+        <v>30</v>
+      </c>
+      <c r="H39" s="29">
+        <v>51</v>
+      </c>
+      <c r="I39" s="29">
+        <v>57</v>
+      </c>
+      <c r="J39" s="61">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A40" s="33">
+        <v>37</v>
+      </c>
+      <c r="B40" s="37">
+        <v>69</v>
+      </c>
+      <c r="C40" s="71">
+        <v>101</v>
+      </c>
+      <c r="D40" s="71">
+        <v>73</v>
+      </c>
+      <c r="E40" s="38">
+        <v>105</v>
+      </c>
+      <c r="F40" s="74"/>
+      <c r="G40" s="58">
+        <v>27</v>
+      </c>
+      <c r="H40" s="29">
+        <v>35</v>
+      </c>
+      <c r="I40" s="29">
+        <v>59</v>
+      </c>
+      <c r="J40" s="61">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A41" s="33">
+        <v>38</v>
+      </c>
+      <c r="B41" s="37">
+        <v>70</v>
+      </c>
+      <c r="C41" s="71">
+        <v>102</v>
+      </c>
+      <c r="D41" s="71">
+        <v>74</v>
+      </c>
+      <c r="E41" s="38">
+        <v>106</v>
+      </c>
+      <c r="F41" s="74"/>
+      <c r="G41" s="58">
+        <v>13</v>
+      </c>
+      <c r="H41" s="29">
+        <v>58</v>
+      </c>
+      <c r="I41" s="29">
+        <v>53</v>
+      </c>
+      <c r="J41" s="61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A42" s="33">
+        <v>39</v>
+      </c>
+      <c r="B42" s="37">
+        <v>71</v>
+      </c>
+      <c r="C42" s="71">
+        <v>103</v>
+      </c>
+      <c r="D42" s="71">
+        <v>75</v>
+      </c>
+      <c r="E42" s="38">
+        <v>107</v>
+      </c>
+      <c r="F42" s="74"/>
+      <c r="G42" s="58">
+        <v>38</v>
+      </c>
+      <c r="H42" s="29">
+        <v>12</v>
+      </c>
+      <c r="I42" s="29">
+        <v>5</v>
+      </c>
+      <c r="J42" s="57"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A43" s="33">
+        <v>40</v>
+      </c>
+      <c r="B43" s="37">
+        <v>72</v>
+      </c>
+      <c r="C43" s="71">
+        <v>104</v>
+      </c>
+      <c r="D43" s="71">
+        <v>76</v>
+      </c>
+      <c r="E43" s="38">
+        <v>108</v>
+      </c>
+      <c r="F43" s="74"/>
+      <c r="G43" s="58">
+        <v>57</v>
+      </c>
+      <c r="H43" s="29">
+        <v>9</v>
+      </c>
+      <c r="I43" s="29">
+        <v>23</v>
+      </c>
+      <c r="J43" s="61">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A44" s="33">
+        <v>41</v>
+      </c>
+      <c r="B44" s="37">
+        <v>80</v>
+      </c>
+      <c r="C44" s="71">
+        <v>112</v>
+      </c>
+      <c r="D44" s="71">
+        <v>84</v>
+      </c>
+      <c r="E44" s="38">
+        <v>116</v>
+      </c>
+      <c r="F44" s="74"/>
+      <c r="G44" s="58">
+        <v>46</v>
+      </c>
+      <c r="H44" s="50"/>
+      <c r="I44" s="29">
+        <v>8</v>
+      </c>
+      <c r="J44" s="57"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A45" s="33">
+        <v>42</v>
+      </c>
+      <c r="B45" s="37">
+        <v>79</v>
+      </c>
+      <c r="C45" s="71">
+        <v>111</v>
+      </c>
+      <c r="D45" s="71">
+        <v>83</v>
+      </c>
+      <c r="E45" s="38">
+        <v>115</v>
+      </c>
+      <c r="F45" s="74"/>
+      <c r="G45" s="58">
+        <v>33</v>
+      </c>
+      <c r="H45" s="50"/>
+      <c r="I45" s="29">
+        <v>39</v>
+      </c>
+      <c r="J45" s="57"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A46" s="33">
+        <v>43</v>
+      </c>
+      <c r="B46" s="37">
+        <v>78</v>
+      </c>
+      <c r="C46" s="71">
+        <v>110</v>
+      </c>
+      <c r="D46" s="71">
+        <v>82</v>
+      </c>
+      <c r="E46" s="38">
+        <v>114</v>
+      </c>
+      <c r="F46" s="74"/>
+      <c r="G46" s="58">
+        <v>49</v>
+      </c>
+      <c r="H46" s="50"/>
+      <c r="I46" s="29">
+        <v>31</v>
+      </c>
+      <c r="J46" s="57"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A47" s="33">
+        <v>44</v>
+      </c>
+      <c r="B47" s="37">
+        <v>77</v>
+      </c>
+      <c r="C47" s="71">
+        <v>109</v>
+      </c>
+      <c r="D47" s="71">
+        <v>81</v>
+      </c>
+      <c r="E47" s="38">
+        <v>113</v>
+      </c>
+      <c r="F47" s="74"/>
+      <c r="G47" s="58">
+        <v>22</v>
+      </c>
+      <c r="H47" s="50"/>
+      <c r="I47" s="29">
+        <v>32</v>
+      </c>
+      <c r="J47" s="57"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A48" s="33">
+        <v>45</v>
+      </c>
+      <c r="B48" s="37">
+        <v>76</v>
+      </c>
+      <c r="C48" s="71">
+        <v>108</v>
+      </c>
+      <c r="D48" s="71">
+        <v>80</v>
+      </c>
+      <c r="E48" s="38">
+        <v>112</v>
+      </c>
+      <c r="F48" s="74"/>
+      <c r="G48" s="58">
+        <v>23</v>
+      </c>
+      <c r="H48" s="29">
+        <v>4</v>
+      </c>
+      <c r="I48" s="29">
+        <v>46</v>
+      </c>
+      <c r="J48" s="57"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A49" s="33">
+        <v>46</v>
+      </c>
+      <c r="B49" s="37">
+        <v>75</v>
+      </c>
+      <c r="C49" s="71">
+        <v>107</v>
+      </c>
+      <c r="D49" s="71">
+        <v>79</v>
+      </c>
+      <c r="E49" s="38">
+        <v>111</v>
+      </c>
+      <c r="F49" s="74"/>
+      <c r="G49" s="58">
+        <v>5</v>
+      </c>
+      <c r="H49" s="50"/>
+      <c r="I49" s="29">
+        <v>33</v>
+      </c>
+      <c r="J49" s="57"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A50" s="33">
+        <v>47</v>
+      </c>
+      <c r="B50" s="37">
+        <v>74</v>
+      </c>
+      <c r="C50" s="71">
+        <v>106</v>
+      </c>
+      <c r="D50" s="71">
+        <v>78</v>
+      </c>
+      <c r="E50" s="38">
+        <v>110</v>
+      </c>
+      <c r="F50" s="74"/>
+      <c r="G50" s="58">
+        <v>53</v>
+      </c>
+      <c r="H50" s="29">
+        <v>3</v>
+      </c>
+      <c r="I50" s="29">
+        <v>49</v>
+      </c>
+      <c r="J50" s="57"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A51" s="33">
+        <v>48</v>
+      </c>
+      <c r="B51" s="37">
+        <v>73</v>
+      </c>
+      <c r="C51" s="71">
+        <v>105</v>
+      </c>
+      <c r="D51" s="71">
+        <v>77</v>
+      </c>
+      <c r="E51" s="38">
+        <v>109</v>
+      </c>
+      <c r="F51" s="74"/>
+      <c r="G51" s="58">
+        <v>59</v>
+      </c>
+      <c r="H51" s="29">
+        <v>15</v>
+      </c>
+      <c r="I51" s="29">
+        <v>22</v>
+      </c>
+      <c r="J51" s="57"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A52" s="33">
+        <v>49</v>
+      </c>
+      <c r="B52" s="37">
+        <v>81</v>
+      </c>
+      <c r="C52" s="71">
+        <v>113</v>
+      </c>
+      <c r="D52" s="71">
+        <v>85</v>
+      </c>
+      <c r="E52" s="38">
+        <v>117</v>
+      </c>
+      <c r="F52" s="74"/>
+      <c r="G52" s="58">
+        <v>32</v>
+      </c>
+      <c r="H52" s="50"/>
+      <c r="I52" s="29">
+        <v>7</v>
+      </c>
+      <c r="J52" s="61">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A53" s="33">
+        <v>50</v>
+      </c>
+      <c r="B53" s="37">
+        <v>82</v>
+      </c>
+      <c r="C53" s="71">
+        <v>114</v>
+      </c>
+      <c r="D53" s="71">
+        <v>86</v>
+      </c>
+      <c r="E53" s="38">
+        <v>118</v>
+      </c>
+      <c r="F53" s="74"/>
+      <c r="G53" s="58">
+        <v>31</v>
+      </c>
+      <c r="H53" s="50"/>
+      <c r="I53" s="29">
+        <v>1</v>
+      </c>
+      <c r="J53" s="61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A54" s="33">
+        <v>51</v>
+      </c>
+      <c r="B54" s="37">
+        <v>83</v>
+      </c>
+      <c r="C54" s="71">
+        <v>115</v>
+      </c>
+      <c r="D54" s="71">
+        <v>87</v>
+      </c>
+      <c r="E54" s="38">
+        <v>119</v>
+      </c>
+      <c r="F54" s="74"/>
+      <c r="G54" s="58">
+        <v>39</v>
+      </c>
+      <c r="H54" s="50"/>
+      <c r="I54" s="29">
+        <v>55</v>
+      </c>
+      <c r="J54" s="61">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A55" s="33">
+        <v>52</v>
+      </c>
+      <c r="B55" s="37">
+        <v>84</v>
+      </c>
+      <c r="C55" s="71">
+        <v>116</v>
+      </c>
+      <c r="D55" s="71">
+        <v>88</v>
+      </c>
+      <c r="E55" s="38">
+        <v>120</v>
+      </c>
+      <c r="F55" s="74"/>
+      <c r="G55" s="58">
+        <v>8</v>
+      </c>
+      <c r="H55" s="50"/>
+      <c r="I55" s="29">
+        <v>50</v>
+      </c>
+      <c r="J55" s="61">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A56" s="33">
+        <v>53</v>
+      </c>
+      <c r="B56" s="37">
+        <v>85</v>
+      </c>
+      <c r="C56" s="71">
+        <v>117</v>
+      </c>
+      <c r="D56" s="71">
+        <v>89</v>
+      </c>
+      <c r="E56" s="38">
+        <v>121</v>
+      </c>
+      <c r="F56" s="74"/>
+      <c r="G56" s="58">
+        <v>7</v>
+      </c>
+      <c r="H56" s="29">
+        <v>17</v>
+      </c>
+      <c r="I56" s="29">
+        <v>45</v>
+      </c>
+      <c r="J56" s="61">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A57" s="33">
+        <v>54</v>
+      </c>
+      <c r="B57" s="37">
+        <v>86</v>
+      </c>
+      <c r="C57" s="71">
+        <v>118</v>
+      </c>
+      <c r="D57" s="71">
+        <v>90</v>
+      </c>
+      <c r="E57" s="38">
+        <v>122</v>
+      </c>
+      <c r="F57" s="74"/>
+      <c r="G57" s="58">
+        <v>1</v>
+      </c>
+      <c r="H57" s="29">
+        <v>2</v>
+      </c>
+      <c r="I57" s="29">
+        <v>36</v>
+      </c>
+      <c r="J57" s="61">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A58" s="33">
+        <v>55</v>
+      </c>
+      <c r="B58" s="37">
+        <v>87</v>
+      </c>
+      <c r="C58" s="71">
+        <v>119</v>
+      </c>
+      <c r="D58" s="71">
+        <v>91</v>
+      </c>
+      <c r="E58" s="38">
+        <v>123</v>
+      </c>
+      <c r="F58" s="74"/>
+      <c r="G58" s="58">
+        <v>55</v>
+      </c>
+      <c r="H58" s="29">
+        <v>16</v>
+      </c>
+      <c r="I58" s="29">
+        <v>14</v>
+      </c>
+      <c r="J58" s="61">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A59" s="33">
+        <v>56</v>
+      </c>
+      <c r="B59" s="37">
+        <v>88</v>
+      </c>
+      <c r="C59" s="71">
+        <v>120</v>
+      </c>
+      <c r="D59" s="71">
+        <v>92</v>
+      </c>
+      <c r="E59" s="38">
+        <v>124</v>
+      </c>
+      <c r="F59" s="74"/>
+      <c r="G59" s="58">
+        <v>50</v>
+      </c>
+      <c r="H59" s="29">
+        <v>11</v>
+      </c>
+      <c r="I59" s="29">
+        <v>25</v>
+      </c>
+      <c r="J59" s="57"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A60" s="33">
+        <v>57</v>
+      </c>
+      <c r="B60" s="37">
+        <v>96</v>
+      </c>
+      <c r="C60" s="71">
+        <v>128</v>
+      </c>
+      <c r="D60" s="71">
+        <v>100</v>
+      </c>
+      <c r="E60" s="38">
+        <v>68</v>
+      </c>
+      <c r="F60" s="74"/>
+      <c r="G60" s="58">
+        <v>48</v>
+      </c>
+      <c r="H60" s="50"/>
+      <c r="I60" s="29">
+        <v>51</v>
+      </c>
+      <c r="J60" s="61">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A61" s="33">
+        <v>58</v>
+      </c>
+      <c r="B61" s="37">
+        <v>95</v>
+      </c>
+      <c r="C61" s="71">
+        <v>127</v>
+      </c>
+      <c r="D61" s="71">
+        <v>99</v>
+      </c>
+      <c r="E61" s="38">
+        <v>67</v>
+      </c>
+      <c r="F61" s="74"/>
+      <c r="G61" s="58">
+        <v>47</v>
+      </c>
+      <c r="H61" s="50"/>
+      <c r="I61" s="29">
+        <v>43</v>
+      </c>
+      <c r="J61" s="61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A62" s="33">
+        <v>59</v>
+      </c>
+      <c r="B62" s="37">
+        <v>94</v>
+      </c>
+      <c r="C62" s="71">
+        <v>126</v>
+      </c>
+      <c r="D62" s="71">
+        <v>98</v>
+      </c>
+      <c r="E62" s="38">
+        <v>66</v>
+      </c>
+      <c r="F62" s="74"/>
+      <c r="G62" s="58">
+        <v>56</v>
+      </c>
+      <c r="H62" s="50"/>
+      <c r="I62" s="50"/>
+      <c r="J62" s="61">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A63" s="33">
+        <v>60</v>
+      </c>
+      <c r="B63" s="37">
+        <v>93</v>
+      </c>
+      <c r="C63" s="71">
+        <v>125</v>
+      </c>
+      <c r="D63" s="71">
+        <v>97</v>
+      </c>
+      <c r="E63" s="38">
+        <v>65</v>
+      </c>
+      <c r="F63" s="74"/>
+      <c r="G63" s="58">
+        <v>20</v>
+      </c>
+      <c r="H63" s="50"/>
+      <c r="I63" s="50"/>
+      <c r="J63" s="61">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A64" s="33">
+        <v>61</v>
+      </c>
+      <c r="B64" s="37">
+        <v>92</v>
+      </c>
+      <c r="C64" s="71">
+        <v>124</v>
+      </c>
+      <c r="D64" s="71">
+        <v>96</v>
+      </c>
+      <c r="E64" s="38">
+        <v>128</v>
+      </c>
+      <c r="F64" s="74"/>
+      <c r="G64" s="58">
+        <v>25</v>
+      </c>
+      <c r="H64" s="50"/>
+      <c r="I64" s="29">
+        <v>48</v>
+      </c>
+      <c r="J64" s="57"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A65" s="33">
+        <v>62</v>
+      </c>
+      <c r="B65" s="37">
+        <v>91</v>
+      </c>
+      <c r="C65" s="71">
+        <v>123</v>
+      </c>
+      <c r="D65" s="71">
+        <v>95</v>
+      </c>
+      <c r="E65" s="38">
+        <v>127</v>
+      </c>
+      <c r="F65" s="74"/>
+      <c r="G65" s="58">
+        <v>14</v>
+      </c>
+      <c r="H65" s="29">
+        <v>10</v>
+      </c>
+      <c r="I65" s="29">
+        <v>47</v>
+      </c>
+      <c r="J65" s="57"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A66" s="33">
+        <v>63</v>
+      </c>
+      <c r="B66" s="37">
+        <v>90</v>
+      </c>
+      <c r="C66" s="71">
+        <v>122</v>
+      </c>
+      <c r="D66" s="71">
+        <v>94</v>
+      </c>
+      <c r="E66" s="38">
+        <v>126</v>
+      </c>
+      <c r="F66" s="74"/>
+      <c r="G66" s="58">
+        <v>36</v>
+      </c>
+      <c r="H66" s="29">
+        <v>24</v>
+      </c>
+      <c r="I66" s="29">
+        <v>56</v>
+      </c>
+      <c r="J66" s="57"/>
+    </row>
+    <row r="67" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A67" s="33">
+        <v>64</v>
+      </c>
+      <c r="B67" s="39">
+        <v>89</v>
+      </c>
+      <c r="C67" s="40">
+        <v>121</v>
+      </c>
+      <c r="D67" s="40">
+        <v>93</v>
+      </c>
+      <c r="E67" s="41">
+        <v>125</v>
+      </c>
+      <c r="F67" s="75"/>
+      <c r="G67" s="70">
+        <v>45</v>
+      </c>
+      <c r="H67" s="62">
+        <v>19</v>
+      </c>
+      <c r="I67" s="62">
+        <v>20</v>
+      </c>
+      <c r="J67" s="63"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="F36:F67"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="F4:F35"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE874426-3D14-41F9-B43B-9BEDEA17B539}">
   <dimension ref="A1:N61"/>
   <sheetViews>
@@ -10117,15 +12244,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AE2369821C535B4A926EDE6FD95680EF" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="25f7092aaaccfe28f06aaa49dbc1c38a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="82955996-2c56-4dc5-a205-5349b3b0490a" xmlns:ns3="f40b0abf-00a2-4b5b-b98d-06c28878d409" xmlns:ns4="eddb54b3-0260-4a74-8bba-cc772719b91b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="30857444423b66cafcc1ac54cc211eeb" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="82955996-2c56-4dc5-a205-5349b3b0490a"/>
@@ -10373,7 +12491,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="f40b0abf-00a2-4b5b-b98d-06c28878d409">
@@ -10391,15 +12509,16 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC23E6A2-90B8-4860-9A82-94B40C6384C0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8054A871-991D-4D18-AE98-F9DEB4B6F288}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10419,7 +12538,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29D9ED97-9FFF-4588-8DC9-F5F025F5C220}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -10429,4 +12548,12 @@
     <ds:schemaRef ds:uri="eddb54b3-0260-4a74-8bba-cc772719b91b"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC23E6A2-90B8-4860-9A82-94B40C6384C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>